<commit_message>
modificaciones menus , warehouse , tailor made
</commit_message>
<xml_diff>
--- a/web/reportes/tracking-1.xlsx
+++ b/web/reportes/tracking-1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4538" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4500" uniqueCount="30">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -862,10 +862,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>41794.85119212963</v>
+        <v>41795.00078703704</v>
       </c>
       <c r="D8" s="16" t="n">
-        <v>41794.85119212963</v>
+        <v>41795.00078703704</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>8</v>
@@ -888,10 +888,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="14" t="n">
-        <v>41794.95861111111</v>
+        <v>41795.001967592594</v>
       </c>
       <c r="D9" s="16" t="n">
-        <v>41794.95861111111</v>
+        <v>41795.001967592594</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>8</v>
@@ -917,10 +917,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="14" t="n">
-        <v>41794.96034722222</v>
+        <v>41795.00362268519</v>
       </c>
       <c r="D10" s="16" t="n">
-        <v>41794.96034722222</v>
+        <v>41795.00362268519</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>8</v>
@@ -943,10 +943,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="14" t="n">
-        <v>41794.96319444444</v>
+        <v>41795.00409722222</v>
       </c>
       <c r="D11" s="16" t="n">
-        <v>41794.96319444444</v>
+        <v>41795.00409722222</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>8</v>
@@ -969,10 +969,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="14" t="n">
-        <v>41794.963796296295</v>
+        <v>41795.004895833335</v>
       </c>
       <c r="D12" s="16" t="n">
-        <v>41794.963796296295</v>
+        <v>41795.004895833335</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>8</v>
@@ -995,10 +995,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="14" t="n">
-        <v>41794.965219907404</v>
+        <v>41795.00578703704</v>
       </c>
       <c r="D13" s="16" t="n">
-        <v>41794.965219907404</v>
+        <v>41795.00578703704</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>8</v>
@@ -1021,10 +1021,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="14" t="n">
-        <v>41794.965787037036</v>
+        <v>41795.007256944446</v>
       </c>
       <c r="D14" s="16" t="n">
-        <v>41794.965787037036</v>
+        <v>41795.007256944446</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>8</v>
@@ -1047,10 +1047,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="14" t="n">
-        <v>41794.968622685185</v>
+        <v>41795.01219907407</v>
       </c>
       <c r="D15" s="16" t="n">
-        <v>41794.968622685185</v>
+        <v>41795.01219907407</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>8</v>
@@ -1073,10 +1073,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>41794.975127314814</v>
+        <v>41795.016805555555</v>
       </c>
       <c r="D16" s="16" t="n">
-        <v>41794.975127314814</v>
+        <v>41795.016805555555</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>8</v>
@@ -1099,10 +1099,10 @@
         <v>7</v>
       </c>
       <c r="C17" s="14" t="n">
-        <v>41794.977060185185</v>
+        <v>41798.49767361111</v>
       </c>
       <c r="D17" s="16" t="n">
-        <v>41794.977060185185</v>
+        <v>41798.49767361111</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>8</v>
@@ -1125,10 +1125,10 @@
         <v>7</v>
       </c>
       <c r="C18" s="14" t="n">
-        <v>41794.97756944445</v>
+        <v>41798.50548611111</v>
       </c>
       <c r="D18" s="16" t="n">
-        <v>41794.97756944445</v>
+        <v>41798.50548611111</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>8</v>
@@ -1151,10 +1151,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="14" t="n">
-        <v>41794.97840277778</v>
+        <v>41798.506064814814</v>
       </c>
       <c r="D19" s="16" t="n">
-        <v>41794.97840277778</v>
+        <v>41798.506064814814</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>8</v>
@@ -1177,10 +1177,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="14" t="n">
-        <v>41794.97920138889</v>
+        <v>41798.51210648148</v>
       </c>
       <c r="D20" s="16" t="n">
-        <v>41794.97920138889</v>
+        <v>41798.51210648148</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>8</v>
@@ -1203,10 +1203,10 @@
         <v>7</v>
       </c>
       <c r="C21" s="14" t="n">
-        <v>41794.98711805556</v>
+        <v>41798.51399305555</v>
       </c>
       <c r="D21" s="16" t="n">
-        <v>41794.98711805556</v>
+        <v>41798.51399305555</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>8</v>
@@ -1229,10 +1229,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="14" t="n">
-        <v>41794.9909375</v>
+        <v>41798.514548611114</v>
       </c>
       <c r="D22" s="16" t="n">
-        <v>41794.9909375</v>
+        <v>41798.514548611114</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>8</v>
@@ -1255,10 +1255,10 @@
         <v>7</v>
       </c>
       <c r="C23" s="14" t="n">
-        <v>41794.992372685185</v>
+        <v>41798.517060185186</v>
       </c>
       <c r="D23" s="16" t="n">
-        <v>41794.992372685185</v>
+        <v>41798.517060185186</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>8</v>
@@ -1281,10 +1281,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="14" t="n">
-        <v>41794.99790509259</v>
+        <v>41798.51924768519</v>
       </c>
       <c r="D24" s="16" t="n">
-        <v>41794.99790509259</v>
+        <v>41798.51924768519</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>8</v>
@@ -1307,10 +1307,10 @@
         <v>7</v>
       </c>
       <c r="C25" s="14" t="n">
-        <v>41794.99880787037</v>
+        <v>41798.519953703704</v>
       </c>
       <c r="D25" s="16" t="n">
-        <v>41794.99880787037</v>
+        <v>41798.519953703704</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>8</v>
@@ -1333,10 +1333,10 @@
         <v>7</v>
       </c>
       <c r="C26" s="14" t="n">
-        <v>41794.99990740741</v>
+        <v>41798.521145833336</v>
       </c>
       <c r="D26" s="16" t="n">
-        <v>41794.99990740741</v>
+        <v>41798.521145833336</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>8</v>
@@ -1359,10 +1359,10 @@
         <v>7</v>
       </c>
       <c r="C27" s="14" t="n">
-        <v>41795.00078703704</v>
+        <v>41798.52226851852</v>
       </c>
       <c r="D27" s="16" t="n">
-        <v>41795.00078703704</v>
+        <v>41798.52226851852</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>8</v>
@@ -1385,10 +1385,10 @@
         <v>7</v>
       </c>
       <c r="C28" s="14" t="n">
-        <v>41795.001967592594</v>
+        <v>41798.523680555554</v>
       </c>
       <c r="D28" s="16" t="n">
-        <v>41795.001967592594</v>
+        <v>41798.523680555554</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>8</v>
@@ -1411,10 +1411,10 @@
         <v>7</v>
       </c>
       <c r="C29" s="14" t="n">
-        <v>41795.00362268519</v>
+        <v>41798.5271875</v>
       </c>
       <c r="D29" s="16" t="n">
-        <v>41795.00362268519</v>
+        <v>41798.5271875</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>8</v>
@@ -1437,10 +1437,10 @@
         <v>7</v>
       </c>
       <c r="C30" s="14" t="n">
-        <v>41795.00409722222</v>
+        <v>41798.54523148148</v>
       </c>
       <c r="D30" s="16" t="n">
-        <v>41795.00409722222</v>
+        <v>41798.54523148148</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>8</v>
@@ -1463,10 +1463,10 @@
         <v>7</v>
       </c>
       <c r="C31" s="14" t="n">
-        <v>41795.004895833335</v>
+        <v>41798.54622685185</v>
       </c>
       <c r="D31" s="16" t="n">
-        <v>41795.004895833335</v>
+        <v>41798.54622685185</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>8</v>
@@ -1489,10 +1489,10 @@
         <v>7</v>
       </c>
       <c r="C32" s="14" t="n">
-        <v>41795.00578703704</v>
+        <v>41798.54702546296</v>
       </c>
       <c r="D32" s="16" t="n">
-        <v>41795.00578703704</v>
+        <v>41798.54702546296</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>8</v>
@@ -1515,10 +1515,10 @@
         <v>7</v>
       </c>
       <c r="C33" s="14" t="n">
-        <v>41795.007256944446</v>
+        <v>41798.547743055555</v>
       </c>
       <c r="D33" s="16" t="n">
-        <v>41795.007256944446</v>
+        <v>41798.547743055555</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>8</v>
@@ -1541,10 +1541,10 @@
         <v>7</v>
       </c>
       <c r="C34" s="14" t="n">
-        <v>41795.01219907407</v>
+        <v>41798.549363425926</v>
       </c>
       <c r="D34" s="16" t="n">
-        <v>41795.01219907407</v>
+        <v>41798.549363425926</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>8</v>
@@ -1567,10 +1567,10 @@
         <v>7</v>
       </c>
       <c r="C35" s="14" t="n">
-        <v>41795.016805555555</v>
+        <v>41798.550208333334</v>
       </c>
       <c r="D35" s="16" t="n">
-        <v>41795.016805555555</v>
+        <v>41798.550208333334</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>8</v>
@@ -1593,10 +1593,10 @@
         <v>7</v>
       </c>
       <c r="C36" s="14" t="n">
-        <v>41798.49767361111</v>
+        <v>41798.55111111111</v>
       </c>
       <c r="D36" s="16" t="n">
-        <v>41798.49767361111</v>
+        <v>41798.55111111111</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>8</v>
@@ -1619,10 +1619,10 @@
         <v>7</v>
       </c>
       <c r="C37" s="14" t="n">
-        <v>41798.50548611111</v>
+        <v>41798.55197916667</v>
       </c>
       <c r="D37" s="16" t="n">
-        <v>41798.50548611111</v>
+        <v>41798.55197916667</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>8</v>
@@ -1645,10 +1645,10 @@
         <v>7</v>
       </c>
       <c r="C38" s="14" t="n">
-        <v>41798.506064814814</v>
+        <v>41798.553449074076</v>
       </c>
       <c r="D38" s="16" t="n">
-        <v>41798.506064814814</v>
+        <v>41798.553449074076</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>8</v>
@@ -1671,10 +1671,10 @@
         <v>7</v>
       </c>
       <c r="C39" s="14" t="n">
-        <v>41798.51210648148</v>
+        <v>41798.55532407408</v>
       </c>
       <c r="D39" s="16" t="n">
-        <v>41798.51210648148</v>
+        <v>41798.55532407408</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>8</v>
@@ -1697,10 +1697,10 @@
         <v>7</v>
       </c>
       <c r="C40" s="14" t="n">
-        <v>41798.51399305555</v>
+        <v>41798.55832175926</v>
       </c>
       <c r="D40" s="16" t="n">
-        <v>41798.51399305555</v>
+        <v>41798.55832175926</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>8</v>
@@ -1723,10 +1723,10 @@
         <v>7</v>
       </c>
       <c r="C41" s="14" t="n">
-        <v>41798.514548611114</v>
+        <v>41798.56319444445</v>
       </c>
       <c r="D41" s="16" t="n">
-        <v>41798.514548611114</v>
+        <v>41798.56319444445</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>8</v>
@@ -1749,10 +1749,10 @@
         <v>7</v>
       </c>
       <c r="C42" s="14" t="n">
-        <v>41798.517060185186</v>
+        <v>41798.564108796294</v>
       </c>
       <c r="D42" s="16" t="n">
-        <v>41798.517060185186</v>
+        <v>41798.564108796294</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>8</v>
@@ -1775,10 +1775,10 @@
         <v>7</v>
       </c>
       <c r="C43" s="14" t="n">
-        <v>41798.51924768519</v>
+        <v>41798.564618055556</v>
       </c>
       <c r="D43" s="16" t="n">
-        <v>41798.51924768519</v>
+        <v>41798.564618055556</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>8</v>
@@ -1801,10 +1801,10 @@
         <v>7</v>
       </c>
       <c r="C44" s="14" t="n">
-        <v>41798.519953703704</v>
+        <v>41798.56903935185</v>
       </c>
       <c r="D44" s="16" t="n">
-        <v>41798.519953703704</v>
+        <v>41798.56903935185</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>8</v>
@@ -1827,10 +1827,10 @@
         <v>7</v>
       </c>
       <c r="C45" s="14" t="n">
-        <v>41798.521145833336</v>
+        <v>41798.56989583333</v>
       </c>
       <c r="D45" s="16" t="n">
-        <v>41798.521145833336</v>
+        <v>41798.56989583333</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>8</v>
@@ -1853,10 +1853,10 @@
         <v>7</v>
       </c>
       <c r="C46" s="14" t="n">
-        <v>41798.52226851852</v>
+        <v>41798.57283564815</v>
       </c>
       <c r="D46" s="16" t="n">
-        <v>41798.52226851852</v>
+        <v>41798.57283564815</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>8</v>
@@ -1879,10 +1879,10 @@
         <v>7</v>
       </c>
       <c r="C47" s="14" t="n">
-        <v>41798.523680555554</v>
+        <v>41798.573483796295</v>
       </c>
       <c r="D47" s="16" t="n">
-        <v>41798.523680555554</v>
+        <v>41798.573483796295</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>8</v>
@@ -1905,10 +1905,10 @@
         <v>7</v>
       </c>
       <c r="C48" s="14" t="n">
-        <v>41798.5271875</v>
+        <v>41798.575324074074</v>
       </c>
       <c r="D48" s="16" t="n">
-        <v>41798.5271875</v>
+        <v>41798.575324074074</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>8</v>
@@ -1931,10 +1931,10 @@
         <v>7</v>
       </c>
       <c r="C49" s="14" t="n">
-        <v>41798.54523148148</v>
+        <v>41798.577199074076</v>
       </c>
       <c r="D49" s="16" t="n">
-        <v>41798.54523148148</v>
+        <v>41798.577199074076</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>8</v>
@@ -1957,10 +1957,10 @@
         <v>7</v>
       </c>
       <c r="C50" s="14" t="n">
-        <v>41798.54622685185</v>
+        <v>41798.579409722224</v>
       </c>
       <c r="D50" s="16" t="n">
-        <v>41798.54622685185</v>
+        <v>41798.579409722224</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>8</v>
@@ -1983,10 +1983,10 @@
         <v>7</v>
       </c>
       <c r="C51" s="14" t="n">
-        <v>41798.54702546296</v>
+        <v>41798.5812037037</v>
       </c>
       <c r="D51" s="16" t="n">
-        <v>41798.54702546296</v>
+        <v>41798.5812037037</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>8</v>
@@ -2009,10 +2009,10 @@
         <v>7</v>
       </c>
       <c r="C52" s="14" t="n">
-        <v>41798.547743055555</v>
+        <v>41798.582708333335</v>
       </c>
       <c r="D52" s="16" t="n">
-        <v>41798.547743055555</v>
+        <v>41798.582708333335</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>8</v>
@@ -2035,10 +2035,10 @@
         <v>7</v>
       </c>
       <c r="C53" s="14" t="n">
-        <v>41798.549363425926</v>
+        <v>41798.58351851852</v>
       </c>
       <c r="D53" s="16" t="n">
-        <v>41798.549363425926</v>
+        <v>41798.58351851852</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>8</v>
@@ -2061,10 +2061,10 @@
         <v>7</v>
       </c>
       <c r="C54" s="14" t="n">
-        <v>41798.550208333334</v>
+        <v>41798.58559027778</v>
       </c>
       <c r="D54" s="16" t="n">
-        <v>41798.550208333334</v>
+        <v>41798.58559027778</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>8</v>
@@ -2087,10 +2087,10 @@
         <v>7</v>
       </c>
       <c r="C55" s="14" t="n">
-        <v>41798.55111111111</v>
+        <v>41798.58615740741</v>
       </c>
       <c r="D55" s="16" t="n">
-        <v>41798.55111111111</v>
+        <v>41798.58615740741</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>8</v>
@@ -2113,10 +2113,10 @@
         <v>7</v>
       </c>
       <c r="C56" s="14" t="n">
-        <v>41798.55197916667</v>
+        <v>41798.58912037037</v>
       </c>
       <c r="D56" s="16" t="n">
-        <v>41798.55197916667</v>
+        <v>41798.58912037037</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>8</v>
@@ -2139,10 +2139,10 @@
         <v>7</v>
       </c>
       <c r="C57" s="14" t="n">
-        <v>41798.553449074076</v>
+        <v>41798.59005787037</v>
       </c>
       <c r="D57" s="16" t="n">
-        <v>41798.553449074076</v>
+        <v>41798.59005787037</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>8</v>
@@ -2165,10 +2165,10 @@
         <v>7</v>
       </c>
       <c r="C58" s="14" t="n">
-        <v>41798.55532407408</v>
+        <v>41798.59258101852</v>
       </c>
       <c r="D58" s="16" t="n">
-        <v>41798.55532407408</v>
+        <v>41798.59258101852</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>8</v>
@@ -2191,10 +2191,10 @@
         <v>7</v>
       </c>
       <c r="C59" s="14" t="n">
-        <v>41798.55832175926</v>
+        <v>41798.59373842592</v>
       </c>
       <c r="D59" s="16" t="n">
-        <v>41798.55832175926</v>
+        <v>41798.59373842592</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>8</v>
@@ -2217,10 +2217,10 @@
         <v>7</v>
       </c>
       <c r="C60" s="14" t="n">
-        <v>41798.56319444445</v>
+        <v>41798.59601851852</v>
       </c>
       <c r="D60" s="16" t="n">
-        <v>41798.56319444445</v>
+        <v>41798.59601851852</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>8</v>
@@ -2243,10 +2243,10 @@
         <v>7</v>
       </c>
       <c r="C61" s="14" t="n">
-        <v>41798.564108796294</v>
+        <v>41798.597025462965</v>
       </c>
       <c r="D61" s="16" t="n">
-        <v>41798.564108796294</v>
+        <v>41798.597025462965</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>8</v>
@@ -2269,10 +2269,10 @@
         <v>7</v>
       </c>
       <c r="C62" s="14" t="n">
-        <v>41798.564618055556</v>
+        <v>41798.61094907407</v>
       </c>
       <c r="D62" s="16" t="n">
-        <v>41798.564618055556</v>
+        <v>41798.61094907407</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>8</v>
@@ -2295,10 +2295,10 @@
         <v>7</v>
       </c>
       <c r="C63" s="14" t="n">
-        <v>41798.56903935185</v>
+        <v>41798.613032407404</v>
       </c>
       <c r="D63" s="16" t="n">
-        <v>41798.56903935185</v>
+        <v>41798.613032407404</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>8</v>
@@ -2321,10 +2321,10 @@
         <v>7</v>
       </c>
       <c r="C64" s="14" t="n">
-        <v>41798.56989583333</v>
+        <v>41798.621099537035</v>
       </c>
       <c r="D64" s="16" t="n">
-        <v>41798.56989583333</v>
+        <v>41798.621099537035</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>8</v>
@@ -2347,10 +2347,10 @@
         <v>7</v>
       </c>
       <c r="C65" s="14" t="n">
-        <v>41798.57283564815</v>
+        <v>41798.62221064815</v>
       </c>
       <c r="D65" s="16" t="n">
-        <v>41798.57283564815</v>
+        <v>41798.62221064815</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>8</v>
@@ -2373,10 +2373,10 @@
         <v>7</v>
       </c>
       <c r="C66" s="14" t="n">
-        <v>41798.573483796295</v>
+        <v>41798.62320601852</v>
       </c>
       <c r="D66" s="16" t="n">
-        <v>41798.573483796295</v>
+        <v>41798.62320601852</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>8</v>
@@ -2399,10 +2399,10 @@
         <v>7</v>
       </c>
       <c r="C67" s="14" t="n">
-        <v>41798.575324074074</v>
+        <v>41798.62384259259</v>
       </c>
       <c r="D67" s="16" t="n">
-        <v>41798.575324074074</v>
+        <v>41798.62384259259</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>8</v>
@@ -2425,10 +2425,10 @@
         <v>7</v>
       </c>
       <c r="C68" s="14" t="n">
-        <v>41798.577199074076</v>
+        <v>41798.62793981482</v>
       </c>
       <c r="D68" s="16" t="n">
-        <v>41798.577199074076</v>
+        <v>41798.62793981482</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>8</v>
@@ -2451,10 +2451,10 @@
         <v>7</v>
       </c>
       <c r="C69" s="14" t="n">
-        <v>41798.579409722224</v>
+        <v>41798.631585648145</v>
       </c>
       <c r="D69" s="16" t="n">
-        <v>41798.579409722224</v>
+        <v>41798.631585648145</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>8</v>
@@ -2477,10 +2477,10 @@
         <v>7</v>
       </c>
       <c r="C70" s="14" t="n">
-        <v>41798.5812037037</v>
+        <v>41798.63246527778</v>
       </c>
       <c r="D70" s="16" t="n">
-        <v>41798.5812037037</v>
+        <v>41798.63246527778</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>8</v>
@@ -2503,10 +2503,10 @@
         <v>7</v>
       </c>
       <c r="C71" s="14" t="n">
-        <v>41798.582708333335</v>
+        <v>41798.63810185185</v>
       </c>
       <c r="D71" s="16" t="n">
-        <v>41798.582708333335</v>
+        <v>41798.63810185185</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>8</v>
@@ -2529,10 +2529,10 @@
         <v>7</v>
       </c>
       <c r="C72" s="14" t="n">
-        <v>41798.58351851852</v>
+        <v>41798.63961805555</v>
       </c>
       <c r="D72" s="16" t="n">
-        <v>41798.58351851852</v>
+        <v>41798.63961805555</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>8</v>
@@ -2555,10 +2555,10 @@
         <v>7</v>
       </c>
       <c r="C73" s="14" t="n">
-        <v>41798.58559027778</v>
+        <v>41798.643379629626</v>
       </c>
       <c r="D73" s="16" t="n">
-        <v>41798.58559027778</v>
+        <v>41798.643379629626</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>8</v>
@@ -2581,13 +2581,13 @@
         <v>7</v>
       </c>
       <c r="C74" s="14" t="n">
-        <v>41798.58615740741</v>
+        <v>41798.64365740741</v>
       </c>
       <c r="D74" s="16" t="n">
-        <v>41798.58615740741</v>
+        <v>41798.64365740741</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F74" s="10">
         <v>0</v>
@@ -2607,10 +2607,10 @@
         <v>7</v>
       </c>
       <c r="C75" s="14" t="n">
-        <v>41798.58912037037</v>
+        <v>41798.67159722222</v>
       </c>
       <c r="D75" s="16" t="n">
-        <v>41798.58912037037</v>
+        <v>41798.67159722222</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>8</v>
@@ -2633,10 +2633,10 @@
         <v>7</v>
       </c>
       <c r="C76" s="14" t="n">
-        <v>41798.59005787037</v>
+        <v>41798.67420138889</v>
       </c>
       <c r="D76" s="16" t="n">
-        <v>41798.59005787037</v>
+        <v>41798.67420138889</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>8</v>
@@ -2659,10 +2659,10 @@
         <v>7</v>
       </c>
       <c r="C77" s="14" t="n">
-        <v>41798.59258101852</v>
+        <v>41798.67643518518</v>
       </c>
       <c r="D77" s="16" t="n">
-        <v>41798.59258101852</v>
+        <v>41798.67643518518</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>8</v>
@@ -2685,10 +2685,10 @@
         <v>7</v>
       </c>
       <c r="C78" s="14" t="n">
-        <v>41798.59373842592</v>
+        <v>41798.6787962963</v>
       </c>
       <c r="D78" s="16" t="n">
-        <v>41798.59373842592</v>
+        <v>41798.6787962963</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>8</v>
@@ -2711,10 +2711,10 @@
         <v>7</v>
       </c>
       <c r="C79" s="14" t="n">
-        <v>41798.59601851852</v>
+        <v>41798.72858796296</v>
       </c>
       <c r="D79" s="16" t="n">
-        <v>41798.59601851852</v>
+        <v>41798.72858796296</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>8</v>
@@ -2737,10 +2737,10 @@
         <v>7</v>
       </c>
       <c r="C80" s="14" t="n">
-        <v>41798.597025462965</v>
+        <v>41798.73149305556</v>
       </c>
       <c r="D80" s="16" t="n">
-        <v>41798.597025462965</v>
+        <v>41798.73149305556</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>8</v>
@@ -2763,10 +2763,10 @@
         <v>7</v>
       </c>
       <c r="C81" s="14" t="n">
-        <v>41798.61094907407</v>
+        <v>41798.73357638889</v>
       </c>
       <c r="D81" s="16" t="n">
-        <v>41798.61094907407</v>
+        <v>41798.73357638889</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>8</v>
@@ -2789,10 +2789,10 @@
         <v>7</v>
       </c>
       <c r="C82" s="14" t="n">
-        <v>41798.613032407404</v>
+        <v>41798.736134259256</v>
       </c>
       <c r="D82" s="16" t="n">
-        <v>41798.613032407404</v>
+        <v>41798.736134259256</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>8</v>
@@ -2815,10 +2815,10 @@
         <v>7</v>
       </c>
       <c r="C83" s="14" t="n">
-        <v>41798.621099537035</v>
+        <v>41798.73755787037</v>
       </c>
       <c r="D83" s="16" t="n">
-        <v>41798.621099537035</v>
+        <v>41798.73755787037</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>8</v>
@@ -2841,10 +2841,10 @@
         <v>7</v>
       </c>
       <c r="C84" s="14" t="n">
-        <v>41798.62221064815</v>
+        <v>41798.740266203706</v>
       </c>
       <c r="D84" s="16" t="n">
-        <v>41798.62221064815</v>
+        <v>41798.740266203706</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>8</v>
@@ -2867,10 +2867,10 @@
         <v>7</v>
       </c>
       <c r="C85" s="14" t="n">
-        <v>41798.62320601852</v>
+        <v>41798.74193287037</v>
       </c>
       <c r="D85" s="16" t="n">
-        <v>41798.62320601852</v>
+        <v>41798.74193287037</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>8</v>
@@ -2893,10 +2893,10 @@
         <v>7</v>
       </c>
       <c r="C86" s="14" t="n">
-        <v>41798.62384259259</v>
+        <v>41798.74386574074</v>
       </c>
       <c r="D86" s="16" t="n">
-        <v>41798.62384259259</v>
+        <v>41798.74386574074</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>8</v>
@@ -2919,10 +2919,10 @@
         <v>7</v>
       </c>
       <c r="C87" s="14" t="n">
-        <v>41798.62793981482</v>
+        <v>41798.84581018519</v>
       </c>
       <c r="D87" s="16" t="n">
-        <v>41798.62793981482</v>
+        <v>41798.84581018519</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>8</v>
@@ -2945,10 +2945,10 @@
         <v>7</v>
       </c>
       <c r="C88" s="14" t="n">
-        <v>41798.631585648145</v>
+        <v>41798.84825231481</v>
       </c>
       <c r="D88" s="16" t="n">
-        <v>41798.631585648145</v>
+        <v>41798.84825231481</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>8</v>
@@ -2971,10 +2971,10 @@
         <v>7</v>
       </c>
       <c r="C89" s="14" t="n">
-        <v>41798.63246527778</v>
+        <v>41798.850266203706</v>
       </c>
       <c r="D89" s="16" t="n">
-        <v>41798.63246527778</v>
+        <v>41798.850266203706</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>8</v>
@@ -2997,10 +2997,10 @@
         <v>7</v>
       </c>
       <c r="C90" s="14" t="n">
-        <v>41798.63810185185</v>
+        <v>41798.98653935185</v>
       </c>
       <c r="D90" s="16" t="n">
-        <v>41798.63810185185</v>
+        <v>41798.98653935185</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>8</v>
@@ -3023,10 +3023,10 @@
         <v>7</v>
       </c>
       <c r="C91" s="14" t="n">
-        <v>41798.63961805555</v>
+        <v>41798.98909722222</v>
       </c>
       <c r="D91" s="16" t="n">
-        <v>41798.63961805555</v>
+        <v>41798.98909722222</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>8</v>
@@ -3049,10 +3049,10 @@
         <v>7</v>
       </c>
       <c r="C92" s="14" t="n">
-        <v>41798.643379629626</v>
+        <v>41798.990891203706</v>
       </c>
       <c r="D92" s="16" t="n">
-        <v>41798.643379629626</v>
+        <v>41798.990891203706</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>8</v>
@@ -3075,13 +3075,13 @@
         <v>7</v>
       </c>
       <c r="C93" s="14" t="n">
-        <v>41798.64365740741</v>
+        <v>41798.99253472222</v>
       </c>
       <c r="D93" s="16" t="n">
-        <v>41798.64365740741</v>
+        <v>41798.99253472222</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" s="10">
         <v>0</v>
@@ -3101,10 +3101,10 @@
         <v>7</v>
       </c>
       <c r="C94" s="14" t="n">
-        <v>41798.67159722222</v>
+        <v>41798.9940162037</v>
       </c>
       <c r="D94" s="16" t="n">
-        <v>41798.67159722222</v>
+        <v>41798.9940162037</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>8</v>
@@ -3127,10 +3127,10 @@
         <v>7</v>
       </c>
       <c r="C95" s="14" t="n">
-        <v>41798.67420138889</v>
+        <v>41798.995150462964</v>
       </c>
       <c r="D95" s="16" t="n">
-        <v>41798.67420138889</v>
+        <v>41798.995150462964</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>8</v>
@@ -3153,10 +3153,10 @@
         <v>7</v>
       </c>
       <c r="C96" s="14" t="n">
-        <v>41798.67643518518</v>
+        <v>41798.99859953704</v>
       </c>
       <c r="D96" s="16" t="n">
-        <v>41798.67643518518</v>
+        <v>41798.99859953704</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>8</v>
@@ -3179,10 +3179,10 @@
         <v>7</v>
       </c>
       <c r="C97" s="14" t="n">
-        <v>41798.6787962963</v>
+        <v>41799.00258101852</v>
       </c>
       <c r="D97" s="16" t="n">
-        <v>41798.6787962963</v>
+        <v>41799.00258101852</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>8</v>
@@ -3205,13 +3205,13 @@
         <v>7</v>
       </c>
       <c r="C98" s="14" t="n">
-        <v>41798.72858796296</v>
+        <v>41799.00273148148</v>
       </c>
       <c r="D98" s="16" t="n">
-        <v>41798.72858796296</v>
+        <v>41799.00273148148</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F98" s="10">
         <v>0</v>
@@ -3231,13 +3231,13 @@
         <v>7</v>
       </c>
       <c r="C99" s="14" t="n">
-        <v>41798.73149305556</v>
+        <v>41799.00293981482</v>
       </c>
       <c r="D99" s="16" t="n">
-        <v>41798.73149305556</v>
+        <v>41799.00293981482</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F99" s="10">
         <v>0</v>
@@ -3257,13 +3257,13 @@
         <v>7</v>
       </c>
       <c r="C100" s="14" t="n">
-        <v>41798.73357638889</v>
+        <v>41799.002962962964</v>
       </c>
       <c r="D100" s="16" t="n">
-        <v>41798.73357638889</v>
+        <v>41799.002962962964</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F100" s="10">
         <v>0</v>
@@ -3283,10 +3283,10 @@
         <v>7</v>
       </c>
       <c r="C101" s="14" t="n">
-        <v>41798.736134259256</v>
+        <v>41799.003113425926</v>
       </c>
       <c r="D101" s="16" t="n">
-        <v>41798.736134259256</v>
+        <v>41799.003113425926</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>8</v>
@@ -3309,13 +3309,13 @@
         <v>7</v>
       </c>
       <c r="C102" s="14" t="n">
-        <v>41798.73755787037</v>
+        <v>41799.00324074074</v>
       </c>
       <c r="D102" s="16" t="n">
-        <v>41798.73755787037</v>
+        <v>41799.00324074074</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F102" s="10">
         <v>0</v>
@@ -3335,13 +3335,13 @@
         <v>7</v>
       </c>
       <c r="C103" s="14" t="n">
-        <v>41798.740266203706</v>
+        <v>41799.003275462965</v>
       </c>
       <c r="D103" s="16" t="n">
-        <v>41798.740266203706</v>
+        <v>41799.003275462965</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F103" s="10">
         <v>0</v>
@@ -3361,10 +3361,10 @@
         <v>7</v>
       </c>
       <c r="C104" s="14" t="n">
-        <v>41798.74193287037</v>
+        <v>41799.957037037035</v>
       </c>
       <c r="D104" s="16" t="n">
-        <v>41798.74193287037</v>
+        <v>41799.957037037035</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>8</v>
@@ -3387,10 +3387,10 @@
         <v>7</v>
       </c>
       <c r="C105" s="14" t="n">
-        <v>41798.74386574074</v>
+        <v>41799.958657407406</v>
       </c>
       <c r="D105" s="16" t="n">
-        <v>41798.74386574074</v>
+        <v>41799.958657407406</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>8</v>
@@ -3413,13 +3413,13 @@
         <v>7</v>
       </c>
       <c r="C106" s="14" t="n">
-        <v>41798.84581018519</v>
+        <v>41799.958969907406</v>
       </c>
       <c r="D106" s="16" t="n">
-        <v>41798.84581018519</v>
+        <v>41799.958969907406</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F106" s="10">
         <v>0</v>
@@ -3439,10 +3439,10 @@
         <v>7</v>
       </c>
       <c r="C107" s="14" t="n">
-        <v>41798.84825231481</v>
+        <v>41799.95998842592</v>
       </c>
       <c r="D107" s="16" t="n">
-        <v>41798.84825231481</v>
+        <v>41799.95998842592</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>8</v>
@@ -3465,13 +3465,13 @@
         <v>7</v>
       </c>
       <c r="C108" s="14" t="n">
-        <v>41798.850266203706</v>
+        <v>41799.96026620371</v>
       </c>
       <c r="D108" s="16" t="n">
-        <v>41798.850266203706</v>
+        <v>41799.96026620371</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F108" s="10">
         <v>0</v>
@@ -3491,13 +3491,13 @@
         <v>7</v>
       </c>
       <c r="C109" s="14" t="n">
-        <v>41798.98653935185</v>
+        <v>41799.96040509259</v>
       </c>
       <c r="D109" s="16" t="n">
-        <v>41798.98653935185</v>
+        <v>41799.96040509259</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F109" s="10">
         <v>0</v>
@@ -3517,10 +3517,10 @@
         <v>7</v>
       </c>
       <c r="C110" s="14" t="n">
-        <v>41798.98909722222</v>
+        <v>41799.9609375</v>
       </c>
       <c r="D110" s="16" t="n">
-        <v>41798.98909722222</v>
+        <v>41799.9609375</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>8</v>
@@ -3543,13 +3543,13 @@
         <v>7</v>
       </c>
       <c r="C111" s="14" t="n">
-        <v>41798.990891203706</v>
+        <v>41799.961388888885</v>
       </c>
       <c r="D111" s="16" t="n">
-        <v>41798.990891203706</v>
+        <v>41799.961388888885</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F111" s="10">
         <v>0</v>
@@ -3569,13 +3569,13 @@
         <v>7</v>
       </c>
       <c r="C112" s="14" t="n">
-        <v>41798.99253472222</v>
+        <v>41799.96141203704</v>
       </c>
       <c r="D112" s="16" t="n">
-        <v>41798.99253472222</v>
+        <v>41799.96141203704</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F112" s="10">
         <v>0</v>
@@ -3595,10 +3595,10 @@
         <v>7</v>
       </c>
       <c r="C113" s="14" t="n">
-        <v>41798.9940162037</v>
+        <v>41799.961481481485</v>
       </c>
       <c r="D113" s="16" t="n">
-        <v>41798.9940162037</v>
+        <v>41799.961481481485</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>8</v>
@@ -3621,13 +3621,13 @@
         <v>7</v>
       </c>
       <c r="C114" s="14" t="n">
-        <v>41798.995150462964</v>
+        <v>41799.96165509259</v>
       </c>
       <c r="D114" s="16" t="n">
-        <v>41798.995150462964</v>
+        <v>41799.96165509259</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F114" s="10">
         <v>0</v>
@@ -3647,13 +3647,13 @@
         <v>7</v>
       </c>
       <c r="C115" s="14" t="n">
-        <v>41798.99859953704</v>
+        <v>41799.96197916667</v>
       </c>
       <c r="D115" s="16" t="n">
-        <v>41798.99859953704</v>
+        <v>41799.96197916667</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F115" s="10">
         <v>0</v>
@@ -3673,10 +3673,10 @@
         <v>7</v>
       </c>
       <c r="C116" s="14" t="n">
-        <v>41799.00258101852</v>
+        <v>41799.979525462964</v>
       </c>
       <c r="D116" s="16" t="n">
-        <v>41799.00258101852</v>
+        <v>41799.979525462964</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>8</v>
@@ -3699,13 +3699,13 @@
         <v>7</v>
       </c>
       <c r="C117" s="14" t="n">
-        <v>41799.00273148148</v>
+        <v>41799.985439814816</v>
       </c>
       <c r="D117" s="16" t="n">
-        <v>41799.00273148148</v>
+        <v>41799.985439814816</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F117" s="10">
         <v>0</v>
@@ -3725,13 +3725,13 @@
         <v>7</v>
       </c>
       <c r="C118" s="14" t="n">
-        <v>41799.00293981482</v>
+        <v>41799.99940972222</v>
       </c>
       <c r="D118" s="16" t="n">
-        <v>41799.00293981482</v>
+        <v>41799.99940972222</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F118" s="10">
         <v>0</v>
@@ -3751,13 +3751,13 @@
         <v>7</v>
       </c>
       <c r="C119" s="14" t="n">
-        <v>41799.002962962964</v>
+        <v>41800.000810185185</v>
       </c>
       <c r="D119" s="16" t="n">
-        <v>41799.002962962964</v>
+        <v>41800.000810185185</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F119" s="10">
         <v>0</v>
@@ -3777,13 +3777,13 @@
         <v>7</v>
       </c>
       <c r="C120" s="14" t="n">
-        <v>41799.003113425926</v>
+        <v>41800.000868055555</v>
       </c>
       <c r="D120" s="16" t="n">
-        <v>41799.003113425926</v>
+        <v>41800.000868055555</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F120" s="10">
         <v>0</v>
@@ -3803,13 +3803,13 @@
         <v>7</v>
       </c>
       <c r="C121" s="14" t="n">
-        <v>41799.00324074074</v>
+        <v>41800.00179398148</v>
       </c>
       <c r="D121" s="16" t="n">
-        <v>41799.00324074074</v>
+        <v>41800.00179398148</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F121" s="10">
         <v>0</v>
@@ -3829,13 +3829,13 @@
         <v>7</v>
       </c>
       <c r="C122" s="14" t="n">
-        <v>41799.003275462965</v>
+        <v>41800.852685185186</v>
       </c>
       <c r="D122" s="16" t="n">
-        <v>41799.003275462965</v>
+        <v>41800.852685185186</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F122" s="10">
         <v>0</v>
@@ -3855,10 +3855,10 @@
         <v>7</v>
       </c>
       <c r="C123" s="14" t="n">
-        <v>41799.957037037035</v>
+        <v>41802.97175925926</v>
       </c>
       <c r="D123" s="16" t="n">
-        <v>41799.957037037035</v>
+        <v>41802.97175925926</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>8</v>
@@ -3881,10 +3881,10 @@
         <v>7</v>
       </c>
       <c r="C124" s="14" t="n">
-        <v>41799.958657407406</v>
+        <v>41802.973078703704</v>
       </c>
       <c r="D124" s="16" t="n">
-        <v>41799.958657407406</v>
+        <v>41802.973078703704</v>
       </c>
       <c r="E124" s="4" t="s">
         <v>8</v>
@@ -3907,13 +3907,13 @@
         <v>7</v>
       </c>
       <c r="C125" s="14" t="n">
-        <v>41799.958969907406</v>
+        <v>41802.98372685185</v>
       </c>
       <c r="D125" s="16" t="n">
-        <v>41799.958969907406</v>
+        <v>41802.98372685185</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F125" s="10">
         <v>0</v>
@@ -3933,10 +3933,10 @@
         <v>7</v>
       </c>
       <c r="C126" s="14" t="n">
-        <v>41799.95998842592</v>
+        <v>41802.9852662037</v>
       </c>
       <c r="D126" s="16" t="n">
-        <v>41799.95998842592</v>
+        <v>41802.9852662037</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>8</v>
@@ -3959,13 +3959,13 @@
         <v>7</v>
       </c>
       <c r="C127" s="14" t="n">
-        <v>41799.96026620371</v>
+        <v>41802.98813657407</v>
       </c>
       <c r="D127" s="16" t="n">
-        <v>41799.96026620371</v>
+        <v>41802.98813657407</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F127" s="10">
         <v>0</v>
@@ -3985,13 +3985,13 @@
         <v>7</v>
       </c>
       <c r="C128" s="14" t="n">
-        <v>41799.96040509259</v>
+        <v>41802.99209490741</v>
       </c>
       <c r="D128" s="16" t="n">
-        <v>41799.96040509259</v>
+        <v>41802.99209490741</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F128" s="10">
         <v>0</v>
@@ -4011,10 +4011,10 @@
         <v>7</v>
       </c>
       <c r="C129" s="14" t="n">
-        <v>41799.9609375</v>
+        <v>41802.996886574074</v>
       </c>
       <c r="D129" s="16" t="n">
-        <v>41799.9609375</v>
+        <v>41802.996886574074</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>8</v>
@@ -4037,13 +4037,13 @@
         <v>7</v>
       </c>
       <c r="C130" s="14" t="n">
-        <v>41799.961388888885</v>
+        <v>41804.51609953704</v>
       </c>
       <c r="D130" s="16" t="n">
-        <v>41799.961388888885</v>
+        <v>41804.51609953704</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F130" s="10">
         <v>0</v>
@@ -4063,13 +4063,13 @@
         <v>7</v>
       </c>
       <c r="C131" s="14" t="n">
-        <v>41799.96141203704</v>
+        <v>41804.524502314816</v>
       </c>
       <c r="D131" s="16" t="n">
-        <v>41799.96141203704</v>
+        <v>41804.524502314816</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F131" s="10">
         <v>0</v>
@@ -4089,13 +4089,13 @@
         <v>7</v>
       </c>
       <c r="C132" s="14" t="n">
-        <v>41799.961481481485</v>
+        <v>41804.52474537037</v>
       </c>
       <c r="D132" s="16" t="n">
-        <v>41799.961481481485</v>
+        <v>41804.52474537037</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F132" s="10">
         <v>0</v>
@@ -4115,13 +4115,13 @@
         <v>7</v>
       </c>
       <c r="C133" s="14" t="n">
-        <v>41799.96165509259</v>
+        <v>41804.52670138889</v>
       </c>
       <c r="D133" s="16" t="n">
-        <v>41799.96165509259</v>
+        <v>41804.52670138889</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F133" s="10">
         <v>0</v>
@@ -4141,10 +4141,10 @@
         <v>7</v>
       </c>
       <c r="C134" s="14" t="n">
-        <v>41799.96197916667</v>
+        <v>41804.526967592596</v>
       </c>
       <c r="D134" s="16" t="n">
-        <v>41799.96197916667</v>
+        <v>41804.526967592596</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>11</v>
@@ -4167,10 +4167,10 @@
         <v>7</v>
       </c>
       <c r="C135" s="14" t="n">
-        <v>41799.979525462964</v>
+        <v>41804.52890046296</v>
       </c>
       <c r="D135" s="16" t="n">
-        <v>41799.979525462964</v>
+        <v>41804.52890046296</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>8</v>
@@ -4193,10 +4193,10 @@
         <v>7</v>
       </c>
       <c r="C136" s="14" t="n">
-        <v>41799.985439814816</v>
+        <v>41806.91587962963</v>
       </c>
       <c r="D136" s="16" t="n">
-        <v>41799.985439814816</v>
+        <v>41806.91587962963</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>8</v>
@@ -4219,10 +4219,10 @@
         <v>7</v>
       </c>
       <c r="C137" s="14" t="n">
-        <v>41799.99940972222</v>
+        <v>41806.91914351852</v>
       </c>
       <c r="D137" s="16" t="n">
-        <v>41799.99940972222</v>
+        <v>41806.91914351852</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>8</v>
@@ -4245,10 +4245,10 @@
         <v>7</v>
       </c>
       <c r="C138" s="14" t="n">
-        <v>41800.000810185185</v>
+        <v>41806.92680555556</v>
       </c>
       <c r="D138" s="16" t="n">
-        <v>41800.000810185185</v>
+        <v>41806.92680555556</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>8</v>
@@ -4271,10 +4271,10 @@
         <v>7</v>
       </c>
       <c r="C139" s="14" t="n">
-        <v>41800.000868055555</v>
+        <v>41806.92697916667</v>
       </c>
       <c r="D139" s="16" t="n">
-        <v>41800.000868055555</v>
+        <v>41806.92697916667</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>11</v>
@@ -4297,10 +4297,10 @@
         <v>7</v>
       </c>
       <c r="C140" s="14" t="n">
-        <v>41800.00179398148</v>
+        <v>41806.92707175926</v>
       </c>
       <c r="D140" s="16" t="n">
-        <v>41800.00179398148</v>
+        <v>41806.92707175926</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>8</v>
@@ -4323,10 +4323,10 @@
         <v>7</v>
       </c>
       <c r="C141" s="14" t="n">
-        <v>41800.852685185186</v>
+        <v>41806.93303240741</v>
       </c>
       <c r="D141" s="16" t="n">
-        <v>41800.852685185186</v>
+        <v>41806.93303240741</v>
       </c>
       <c r="E141" s="4" t="s">
         <v>8</v>
@@ -4349,13 +4349,13 @@
         <v>7</v>
       </c>
       <c r="C142" s="14" t="n">
-        <v>41802.97175925926</v>
+        <v>41806.93318287037</v>
       </c>
       <c r="D142" s="16" t="n">
-        <v>41802.97175925926</v>
+        <v>41806.93318287037</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F142" s="10">
         <v>0</v>
@@ -4375,10 +4375,10 @@
         <v>7</v>
       </c>
       <c r="C143" s="14" t="n">
-        <v>41802.973078703704</v>
+        <v>41806.93561342593</v>
       </c>
       <c r="D143" s="16" t="n">
-        <v>41802.973078703704</v>
+        <v>41806.93561342593</v>
       </c>
       <c r="E143" s="4" t="s">
         <v>8</v>
@@ -4401,13 +4401,13 @@
         <v>7</v>
       </c>
       <c r="C144" s="14" t="n">
-        <v>41802.98372685185</v>
+        <v>41806.93587962963</v>
       </c>
       <c r="D144" s="16" t="n">
-        <v>41802.98372685185</v>
+        <v>41806.93587962963</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F144" s="10">
         <v>0</v>
@@ -4427,10 +4427,10 @@
         <v>7</v>
       </c>
       <c r="C145" s="14" t="n">
-        <v>41802.9852662037</v>
+        <v>41806.93671296296</v>
       </c>
       <c r="D145" s="16" t="n">
-        <v>41802.9852662037</v>
+        <v>41806.93671296296</v>
       </c>
       <c r="E145" s="4" t="s">
         <v>8</v>
@@ -4453,10 +4453,10 @@
         <v>7</v>
       </c>
       <c r="C146" s="14" t="n">
-        <v>41802.98813657407</v>
+        <v>41806.94064814815</v>
       </c>
       <c r="D146" s="16" t="n">
-        <v>41802.98813657407</v>
+        <v>41806.94064814815</v>
       </c>
       <c r="E146" s="4" t="s">
         <v>8</v>
@@ -4479,10 +4479,10 @@
         <v>7</v>
       </c>
       <c r="C147" s="14" t="n">
-        <v>41802.99209490741</v>
+        <v>41806.94326388889</v>
       </c>
       <c r="D147" s="16" t="n">
-        <v>41802.99209490741</v>
+        <v>41806.94326388889</v>
       </c>
       <c r="E147" s="4" t="s">
         <v>8</v>
@@ -4505,10 +4505,10 @@
         <v>7</v>
       </c>
       <c r="C148" s="14" t="n">
-        <v>41802.996886574074</v>
+        <v>41806.9534375</v>
       </c>
       <c r="D148" s="16" t="n">
-        <v>41802.996886574074</v>
+        <v>41806.9534375</v>
       </c>
       <c r="E148" s="4" t="s">
         <v>8</v>
@@ -4531,13 +4531,13 @@
         <v>7</v>
       </c>
       <c r="C149" s="14" t="n">
-        <v>41804.51609953704</v>
+        <v>41806.95380787037</v>
       </c>
       <c r="D149" s="16" t="n">
-        <v>41804.51609953704</v>
+        <v>41806.95380787037</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F149" s="10">
         <v>0</v>
@@ -4557,13 +4557,13 @@
         <v>7</v>
       </c>
       <c r="C150" s="14" t="n">
-        <v>41804.524502314816</v>
+        <v>41806.95386574074</v>
       </c>
       <c r="D150" s="16" t="n">
-        <v>41804.524502314816</v>
+        <v>41806.95386574074</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F150" s="10">
         <v>0</v>
@@ -4583,13 +4583,13 @@
         <v>7</v>
       </c>
       <c r="C151" s="14" t="n">
-        <v>41804.52474537037</v>
+        <v>41806.95394675926</v>
       </c>
       <c r="D151" s="16" t="n">
-        <v>41804.52474537037</v>
+        <v>41806.95394675926</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F151" s="10">
         <v>0</v>
@@ -4609,13 +4609,13 @@
         <v>7</v>
       </c>
       <c r="C152" s="14" t="n">
-        <v>41804.52670138889</v>
+        <v>41806.95758101852</v>
       </c>
       <c r="D152" s="16" t="n">
-        <v>41804.52670138889</v>
+        <v>41806.95758101852</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F152" s="10">
         <v>0</v>
@@ -4635,10 +4635,10 @@
         <v>7</v>
       </c>
       <c r="C153" s="14" t="n">
-        <v>41804.526967592596</v>
+        <v>41806.95767361111</v>
       </c>
       <c r="D153" s="16" t="n">
-        <v>41804.526967592596</v>
+        <v>41806.95767361111</v>
       </c>
       <c r="E153" s="4" t="s">
         <v>11</v>
@@ -4661,10 +4661,10 @@
         <v>7</v>
       </c>
       <c r="C154" s="14" t="n">
-        <v>41804.52890046296</v>
+        <v>41806.95930555555</v>
       </c>
       <c r="D154" s="16" t="n">
-        <v>41804.52890046296</v>
+        <v>41806.95930555555</v>
       </c>
       <c r="E154" s="4" t="s">
         <v>8</v>
@@ -4687,13 +4687,13 @@
         <v>7</v>
       </c>
       <c r="C155" s="14" t="n">
-        <v>41806.91587962963</v>
+        <v>41806.959444444445</v>
       </c>
       <c r="D155" s="16" t="n">
-        <v>41806.91587962963</v>
+        <v>41806.959444444445</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F155" s="10">
         <v>0</v>
@@ -4713,10 +4713,10 @@
         <v>7</v>
       </c>
       <c r="C156" s="14" t="n">
-        <v>41806.91914351852</v>
+        <v>41806.96302083333</v>
       </c>
       <c r="D156" s="16" t="n">
-        <v>41806.91914351852</v>
+        <v>41806.96302083333</v>
       </c>
       <c r="E156" s="4" t="s">
         <v>8</v>
@@ -4739,10 +4739,10 @@
         <v>7</v>
       </c>
       <c r="C157" s="14" t="n">
-        <v>41806.92680555556</v>
+        <v>41806.964907407404</v>
       </c>
       <c r="D157" s="16" t="n">
-        <v>41806.92680555556</v>
+        <v>41806.964907407404</v>
       </c>
       <c r="E157" s="4" t="s">
         <v>8</v>
@@ -4765,13 +4765,13 @@
         <v>7</v>
       </c>
       <c r="C158" s="14" t="n">
-        <v>41806.92697916667</v>
+        <v>41806.9653125</v>
       </c>
       <c r="D158" s="16" t="n">
-        <v>41806.92697916667</v>
+        <v>41806.9653125</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F158" s="10">
         <v>0</v>
@@ -4791,13 +4791,13 @@
         <v>7</v>
       </c>
       <c r="C159" s="14" t="n">
-        <v>41806.92707175926</v>
+        <v>41806.96542824074</v>
       </c>
       <c r="D159" s="16" t="n">
-        <v>41806.92707175926</v>
+        <v>41806.96542824074</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F159" s="10">
         <v>0</v>
@@ -4817,13 +4817,13 @@
         <v>7</v>
       </c>
       <c r="C160" s="14" t="n">
-        <v>41806.93303240741</v>
+        <v>41806.96545138889</v>
       </c>
       <c r="D160" s="16" t="n">
-        <v>41806.93303240741</v>
+        <v>41806.96545138889</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F160" s="10">
         <v>0</v>
@@ -4840,16 +4840,16 @@
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B161" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C161" s="14" t="n">
-        <v>41806.93318287037</v>
+        <v>41806.96549768518</v>
       </c>
       <c r="D161" s="16" t="n">
-        <v>41806.93318287037</v>
+        <v>41806.96549768518</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F161" s="10">
         <v>0</v>
@@ -4866,16 +4866,16 @@
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B162" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C162" s="14" t="n">
-        <v>41806.93561342593</v>
+        <v>41806.96561342593</v>
       </c>
       <c r="D162" s="16" t="n">
-        <v>41806.93561342593</v>
+        <v>41806.96561342593</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F162" s="10">
         <v>0</v>
@@ -4895,13 +4895,13 @@
         <v>7</v>
       </c>
       <c r="C163" s="14" t="n">
-        <v>41806.93587962963</v>
+        <v>41806.9656712963</v>
       </c>
       <c r="D163" s="16" t="n">
-        <v>41806.93587962963</v>
+        <v>41806.9656712963</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F163" s="10">
         <v>0</v>
@@ -4921,13 +4921,13 @@
         <v>7</v>
       </c>
       <c r="C164" s="14" t="n">
-        <v>41806.93671296296</v>
+        <v>41806.965891203705</v>
       </c>
       <c r="D164" s="16" t="n">
-        <v>41806.93671296296</v>
+        <v>41806.965891203705</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F164" s="10">
         <v>0</v>
@@ -4947,13 +4947,13 @@
         <v>7</v>
       </c>
       <c r="C165" s="14" t="n">
-        <v>41806.94064814815</v>
+        <v>41806.96601851852</v>
       </c>
       <c r="D165" s="16" t="n">
-        <v>41806.94064814815</v>
+        <v>41806.96601851852</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F165" s="10">
         <v>0</v>
@@ -4973,10 +4973,10 @@
         <v>7</v>
       </c>
       <c r="C166" s="14" t="n">
-        <v>41806.94326388889</v>
+        <v>41806.966261574074</v>
       </c>
       <c r="D166" s="16" t="n">
-        <v>41806.94326388889</v>
+        <v>41806.966261574074</v>
       </c>
       <c r="E166" s="4" t="s">
         <v>8</v>
@@ -4999,13 +4999,13 @@
         <v>7</v>
       </c>
       <c r="C167" s="14" t="n">
-        <v>41806.9534375</v>
+        <v>41806.96681712963</v>
       </c>
       <c r="D167" s="16" t="n">
-        <v>41806.9534375</v>
+        <v>41806.96681712963</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F167" s="10">
         <v>0</v>
@@ -5025,13 +5025,13 @@
         <v>7</v>
       </c>
       <c r="C168" s="14" t="n">
-        <v>41806.95380787037</v>
+        <v>41806.96957175926</v>
       </c>
       <c r="D168" s="16" t="n">
-        <v>41806.95380787037</v>
+        <v>41806.96957175926</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F168" s="10">
         <v>0</v>
@@ -5051,13 +5051,13 @@
         <v>7</v>
       </c>
       <c r="C169" s="14" t="n">
-        <v>41806.95386574074</v>
+        <v>41806.9696875</v>
       </c>
       <c r="D169" s="16" t="n">
-        <v>41806.95386574074</v>
+        <v>41806.9696875</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F169" s="10">
         <v>0</v>
@@ -5077,10 +5077,10 @@
         <v>7</v>
       </c>
       <c r="C170" s="14" t="n">
-        <v>41806.95394675926</v>
+        <v>41806.9699537037</v>
       </c>
       <c r="D170" s="16" t="n">
-        <v>41806.95394675926</v>
+        <v>41806.9699537037</v>
       </c>
       <c r="E170" s="4" t="s">
         <v>11</v>
@@ -5103,10 +5103,10 @@
         <v>7</v>
       </c>
       <c r="C171" s="14" t="n">
-        <v>41806.95758101852</v>
+        <v>41806.97740740741</v>
       </c>
       <c r="D171" s="16" t="n">
-        <v>41806.95758101852</v>
+        <v>41806.97740740741</v>
       </c>
       <c r="E171" s="4" t="s">
         <v>8</v>
@@ -5129,13 +5129,13 @@
         <v>7</v>
       </c>
       <c r="C172" s="14" t="n">
-        <v>41806.95767361111</v>
+        <v>41806.97760416667</v>
       </c>
       <c r="D172" s="16" t="n">
-        <v>41806.95767361111</v>
+        <v>41806.97760416667</v>
       </c>
       <c r="E172" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F172" s="10">
         <v>0</v>
@@ -5155,13 +5155,13 @@
         <v>7</v>
       </c>
       <c r="C173" s="14" t="n">
-        <v>41806.95930555555</v>
+        <v>41806.977638888886</v>
       </c>
       <c r="D173" s="16" t="n">
-        <v>41806.95930555555</v>
+        <v>41806.977638888886</v>
       </c>
       <c r="E173" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F173" s="10">
         <v>0</v>
@@ -5181,13 +5181,13 @@
         <v>7</v>
       </c>
       <c r="C174" s="14" t="n">
-        <v>41806.959444444445</v>
+        <v>41806.97872685185</v>
       </c>
       <c r="D174" s="16" t="n">
-        <v>41806.959444444445</v>
+        <v>41806.97872685185</v>
       </c>
       <c r="E174" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F174" s="10">
         <v>0</v>
@@ -5207,13 +5207,13 @@
         <v>7</v>
       </c>
       <c r="C175" s="14" t="n">
-        <v>41806.96302083333</v>
+        <v>41806.97886574074</v>
       </c>
       <c r="D175" s="16" t="n">
-        <v>41806.96302083333</v>
+        <v>41806.97886574074</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F175" s="10">
         <v>0</v>
@@ -5233,13 +5233,13 @@
         <v>7</v>
       </c>
       <c r="C176" s="14" t="n">
-        <v>41806.964907407404</v>
+        <v>41806.97893518519</v>
       </c>
       <c r="D176" s="16" t="n">
-        <v>41806.964907407404</v>
+        <v>41806.97893518519</v>
       </c>
       <c r="E176" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F176" s="10">
         <v>0</v>
@@ -5256,16 +5256,16 @@
     </row>
     <row r="177" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B177" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C177" s="14" t="n">
-        <v>41806.9653125</v>
+        <v>41806.978993055556</v>
       </c>
       <c r="D177" s="16" t="n">
-        <v>41806.9653125</v>
+        <v>41806.978993055556</v>
       </c>
       <c r="E177" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F177" s="10">
         <v>0</v>
@@ -5282,16 +5282,16 @@
     </row>
     <row r="178" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B178" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C178" s="14" t="n">
-        <v>41806.96542824074</v>
+        <v>41806.97902777778</v>
       </c>
       <c r="D178" s="16" t="n">
-        <v>41806.96542824074</v>
+        <v>41806.97902777778</v>
       </c>
       <c r="E178" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F178" s="10">
         <v>0</v>
@@ -5311,13 +5311,13 @@
         <v>7</v>
       </c>
       <c r="C179" s="14" t="n">
-        <v>41806.96545138889</v>
+        <v>41806.97907407407</v>
       </c>
       <c r="D179" s="16" t="n">
-        <v>41806.96545138889</v>
+        <v>41806.97907407407</v>
       </c>
       <c r="E179" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F179" s="10">
         <v>0</v>
@@ -5334,16 +5334,16 @@
     </row>
     <row r="180" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B180" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C180" s="14" t="n">
-        <v>41806.96549768518</v>
+        <v>41806.97917824074</v>
       </c>
       <c r="D180" s="16" t="n">
-        <v>41806.96549768518</v>
+        <v>41806.97917824074</v>
       </c>
       <c r="E180" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F180" s="10">
         <v>0</v>
@@ -5360,16 +5360,16 @@
     </row>
     <row r="181" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B181" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C181" s="14" t="n">
-        <v>41806.96561342593</v>
+        <v>41806.97918981482</v>
       </c>
       <c r="D181" s="16" t="n">
-        <v>41806.96561342593</v>
+        <v>41806.97918981482</v>
       </c>
       <c r="E181" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F181" s="10">
         <v>0</v>
@@ -5389,10 +5389,10 @@
         <v>7</v>
       </c>
       <c r="C182" s="14" t="n">
-        <v>41806.9656712963</v>
+        <v>41806.98150462963</v>
       </c>
       <c r="D182" s="16" t="n">
-        <v>41806.9656712963</v>
+        <v>41806.98150462963</v>
       </c>
       <c r="E182" s="4" t="s">
         <v>8</v>
@@ -5415,13 +5415,13 @@
         <v>7</v>
       </c>
       <c r="C183" s="14" t="n">
-        <v>41806.965891203705</v>
+        <v>41806.981828703705</v>
       </c>
       <c r="D183" s="16" t="n">
-        <v>41806.965891203705</v>
+        <v>41806.981828703705</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F183" s="10">
         <v>0</v>
@@ -5441,13 +5441,13 @@
         <v>7</v>
       </c>
       <c r="C184" s="14" t="n">
-        <v>41806.96601851852</v>
+        <v>41806.981886574074</v>
       </c>
       <c r="D184" s="16" t="n">
-        <v>41806.96601851852</v>
+        <v>41806.981886574074</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F184" s="10">
         <v>0</v>
@@ -5467,13 +5467,13 @@
         <v>7</v>
       </c>
       <c r="C185" s="14" t="n">
-        <v>41806.966261574074</v>
+        <v>41806.982152777775</v>
       </c>
       <c r="D185" s="16" t="n">
-        <v>41806.966261574074</v>
+        <v>41806.982152777775</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F185" s="10">
         <v>0</v>
@@ -5493,13 +5493,13 @@
         <v>7</v>
       </c>
       <c r="C186" s="14" t="n">
-        <v>41806.96681712963</v>
+        <v>41806.98974537037</v>
       </c>
       <c r="D186" s="16" t="n">
-        <v>41806.96681712963</v>
+        <v>41806.98974537037</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F186" s="10">
         <v>0</v>
@@ -5519,10 +5519,10 @@
         <v>7</v>
       </c>
       <c r="C187" s="14" t="n">
-        <v>41806.96957175926</v>
+        <v>41806.9999537037</v>
       </c>
       <c r="D187" s="16" t="n">
-        <v>41806.96957175926</v>
+        <v>41806.9999537037</v>
       </c>
       <c r="E187" s="4" t="s">
         <v>8</v>
@@ -5545,13 +5545,13 @@
         <v>7</v>
       </c>
       <c r="C188" s="14" t="n">
-        <v>41806.9696875</v>
+        <v>41807.005960648145</v>
       </c>
       <c r="D188" s="16" t="n">
-        <v>41806.9696875</v>
+        <v>41807.005960648145</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F188" s="10">
         <v>0</v>
@@ -5571,13 +5571,13 @@
         <v>7</v>
       </c>
       <c r="C189" s="14" t="n">
-        <v>41806.9699537037</v>
+        <v>41807.00616898148</v>
       </c>
       <c r="D189" s="16" t="n">
-        <v>41806.9699537037</v>
+        <v>41807.00616898148</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F189" s="10">
         <v>0</v>
@@ -5597,13 +5597,13 @@
         <v>7</v>
       </c>
       <c r="C190" s="14" t="n">
-        <v>41806.97740740741</v>
+        <v>41807.00625</v>
       </c>
       <c r="D190" s="16" t="n">
-        <v>41806.97740740741</v>
+        <v>41807.00625</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F190" s="10">
         <v>0</v>
@@ -5623,13 +5623,13 @@
         <v>7</v>
       </c>
       <c r="C191" s="14" t="n">
-        <v>41806.97760416667</v>
+        <v>41807.00628472222</v>
       </c>
       <c r="D191" s="16" t="n">
-        <v>41806.97760416667</v>
+        <v>41807.00628472222</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F191" s="10">
         <v>0</v>
@@ -5646,16 +5646,16 @@
     </row>
     <row r="192" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B192" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C192" s="14" t="n">
-        <v>41806.977638888886</v>
+        <v>41807.00633101852</v>
       </c>
       <c r="D192" s="16" t="n">
-        <v>41806.977638888886</v>
+        <v>41807.00633101852</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F192" s="10">
         <v>0</v>
@@ -5672,16 +5672,16 @@
     </row>
     <row r="193" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B193" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C193" s="14" t="n">
-        <v>41806.97872685185</v>
+        <v>41807.00646990741</v>
       </c>
       <c r="D193" s="16" t="n">
-        <v>41806.97872685185</v>
+        <v>41807.00646990741</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F193" s="10">
         <v>0</v>
@@ -5701,13 +5701,13 @@
         <v>7</v>
       </c>
       <c r="C194" s="14" t="n">
-        <v>41806.97886574074</v>
+        <v>41807.00885416667</v>
       </c>
       <c r="D194" s="16" t="n">
-        <v>41806.97886574074</v>
+        <v>41807.00885416667</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F194" s="10">
         <v>0</v>
@@ -5727,10 +5727,10 @@
         <v>7</v>
       </c>
       <c r="C195" s="14" t="n">
-        <v>41806.97893518519</v>
+        <v>41807.00913194445</v>
       </c>
       <c r="D195" s="16" t="n">
-        <v>41806.97893518519</v>
+        <v>41807.00913194445</v>
       </c>
       <c r="E195" s="4" t="s">
         <v>11</v>
@@ -5750,16 +5750,16 @@
     </row>
     <row r="196" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B196" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C196" s="14" t="n">
-        <v>41806.978993055556</v>
+        <v>41807.014918981484</v>
       </c>
       <c r="D196" s="16" t="n">
-        <v>41806.978993055556</v>
+        <v>41807.014918981484</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F196" s="10">
         <v>0</v>
@@ -5776,16 +5776,16 @@
     </row>
     <row r="197" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B197" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C197" s="14" t="n">
-        <v>41806.97902777778</v>
+        <v>41807.02423611111</v>
       </c>
       <c r="D197" s="16" t="n">
-        <v>41806.97902777778</v>
+        <v>41807.02423611111</v>
       </c>
       <c r="E197" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F197" s="10">
         <v>0</v>
@@ -5802,16 +5802,16 @@
     </row>
     <row r="198" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B198" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C198" s="14" t="n">
-        <v>41806.97907407407</v>
+        <v>41807.027083333334</v>
       </c>
       <c r="D198" s="16" t="n">
-        <v>41806.97907407407</v>
+        <v>41807.027083333334</v>
       </c>
       <c r="E198" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F198" s="10">
         <v>0</v>
@@ -5831,13 +5831,13 @@
         <v>7</v>
       </c>
       <c r="C199" s="14" t="n">
-        <v>41806.97917824074</v>
+        <v>41807.03873842592</v>
       </c>
       <c r="D199" s="16" t="n">
-        <v>41806.97917824074</v>
+        <v>41807.03873842592</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F199" s="10">
         <v>0</v>
@@ -5857,13 +5857,13 @@
         <v>7</v>
       </c>
       <c r="C200" s="14" t="n">
-        <v>41806.97918981482</v>
+        <v>41807.04425925926</v>
       </c>
       <c r="D200" s="16" t="n">
-        <v>41806.97918981482</v>
+        <v>41807.04425925926</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F200" s="10">
         <v>0</v>
@@ -5883,10 +5883,10 @@
         <v>7</v>
       </c>
       <c r="C201" s="14" t="n">
-        <v>41806.98150462963</v>
+        <v>41807.04614583333</v>
       </c>
       <c r="D201" s="16" t="n">
-        <v>41806.98150462963</v>
+        <v>41807.04614583333</v>
       </c>
       <c r="E201" s="4" t="s">
         <v>8</v>
@@ -5906,16 +5906,16 @@
     </row>
     <row r="202" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B202" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C202" s="14" t="n">
-        <v>41806.981828703705</v>
+        <v>41807.0540625</v>
       </c>
       <c r="D202" s="16" t="n">
-        <v>41806.981828703705</v>
+        <v>41807.0540625</v>
       </c>
       <c r="E202" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F202" s="10">
         <v>0</v>
@@ -5932,16 +5932,16 @@
     </row>
     <row r="203" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B203" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C203" s="14" t="n">
-        <v>41806.981886574074</v>
+        <v>41807.05454861111</v>
       </c>
       <c r="D203" s="16" t="n">
-        <v>41806.981886574074</v>
+        <v>41807.05454861111</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F203" s="10">
         <v>0</v>
@@ -5958,16 +5958,16 @@
     </row>
     <row r="204" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B204" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C204" s="14" t="n">
-        <v>41806.982152777775</v>
+        <v>41807.0553125</v>
       </c>
       <c r="D204" s="16" t="n">
-        <v>41806.982152777775</v>
+        <v>41807.0553125</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F204" s="10">
         <v>0</v>
@@ -5984,16 +5984,16 @@
     </row>
     <row r="205" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B205" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C205" s="14" t="n">
-        <v>41806.98974537037</v>
+        <v>41807.056550925925</v>
       </c>
       <c r="D205" s="16" t="n">
-        <v>41806.98974537037</v>
+        <v>41807.056550925925</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="F205" s="10">
         <v>0</v>
@@ -6010,16 +6010,16 @@
     </row>
     <row r="206" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B206" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C206" s="14" t="n">
-        <v>41806.9999537037</v>
+        <v>41807.057974537034</v>
       </c>
       <c r="D206" s="16" t="n">
-        <v>41806.9999537037</v>
+        <v>41807.057974537034</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F206" s="10">
         <v>0</v>
@@ -6036,16 +6036,16 @@
     </row>
     <row r="207" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B207" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C207" s="14" t="n">
-        <v>41807.005960648145</v>
+        <v>41807.0580787037</v>
       </c>
       <c r="D207" s="16" t="n">
-        <v>41807.005960648145</v>
+        <v>41807.0580787037</v>
       </c>
       <c r="E207" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F207" s="10">
         <v>0</v>
@@ -6062,16 +6062,16 @@
     </row>
     <row r="208" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B208" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C208" s="14" t="n">
-        <v>41807.00616898148</v>
+        <v>41807.05868055556</v>
       </c>
       <c r="D208" s="16" t="n">
-        <v>41807.00616898148</v>
+        <v>41807.05868055556</v>
       </c>
       <c r="E208" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F208" s="10">
         <v>0</v>
@@ -6091,13 +6091,13 @@
         <v>7</v>
       </c>
       <c r="C209" s="14" t="n">
-        <v>41807.00625</v>
+        <v>41807.06298611111</v>
       </c>
       <c r="D209" s="16" t="n">
-        <v>41807.00625</v>
+        <v>41807.06298611111</v>
       </c>
       <c r="E209" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F209" s="10">
         <v>0</v>
@@ -6117,13 +6117,13 @@
         <v>7</v>
       </c>
       <c r="C210" s="14" t="n">
-        <v>41807.00628472222</v>
+        <v>41807.06392361111</v>
       </c>
       <c r="D210" s="16" t="n">
-        <v>41807.00628472222</v>
+        <v>41807.06392361111</v>
       </c>
       <c r="E210" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F210" s="10">
         <v>0</v>
@@ -6140,16 +6140,16 @@
     </row>
     <row r="211" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B211" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C211" s="14" t="n">
-        <v>41807.00633101852</v>
+        <v>41807.06418981482</v>
       </c>
       <c r="D211" s="16" t="n">
-        <v>41807.00633101852</v>
+        <v>41807.06418981482</v>
       </c>
       <c r="E211" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F211" s="10">
         <v>0</v>
@@ -6166,16 +6166,16 @@
     </row>
     <row r="212" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B212" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C212" s="14" t="n">
-        <v>41807.00646990741</v>
+        <v>41807.32502314815</v>
       </c>
       <c r="D212" s="16" t="n">
-        <v>41807.00646990741</v>
+        <v>41807.32502314815</v>
       </c>
       <c r="E212" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F212" s="10">
         <v>0</v>
@@ -6195,10 +6195,10 @@
         <v>7</v>
       </c>
       <c r="C213" s="14" t="n">
-        <v>41807.00885416667</v>
+        <v>41807.879791666666</v>
       </c>
       <c r="D213" s="16" t="n">
-        <v>41807.00885416667</v>
+        <v>41807.879791666666</v>
       </c>
       <c r="E213" s="4" t="s">
         <v>8</v>
@@ -6221,13 +6221,13 @@
         <v>7</v>
       </c>
       <c r="C214" s="14" t="n">
-        <v>41807.00913194445</v>
+        <v>41807.88081018518</v>
       </c>
       <c r="D214" s="16" t="n">
-        <v>41807.00913194445</v>
+        <v>41807.88081018518</v>
       </c>
       <c r="E214" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F214" s="10">
         <v>0</v>
@@ -6244,16 +6244,16 @@
     </row>
     <row r="215" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B215" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C215" s="14" t="n">
-        <v>41807.014918981484</v>
+        <v>41807.88452546296</v>
       </c>
       <c r="D215" s="16" t="n">
-        <v>41807.014918981484</v>
+        <v>41807.88452546296</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F215" s="10">
         <v>0</v>
@@ -6273,10 +6273,10 @@
         <v>7</v>
       </c>
       <c r="C216" s="14" t="n">
-        <v>41807.02423611111</v>
+        <v>41807.88659722222</v>
       </c>
       <c r="D216" s="16" t="n">
-        <v>41807.02423611111</v>
+        <v>41807.88659722222</v>
       </c>
       <c r="E216" s="4" t="s">
         <v>8</v>
@@ -6296,16 +6296,16 @@
     </row>
     <row r="217" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B217" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C217" s="14" t="n">
-        <v>41807.027083333334</v>
+        <v>41807.88744212963</v>
       </c>
       <c r="D217" s="16" t="n">
-        <v>41807.027083333334</v>
+        <v>41807.88744212963</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F217" s="10">
         <v>0</v>
@@ -6325,10 +6325,10 @@
         <v>7</v>
       </c>
       <c r="C218" s="14" t="n">
-        <v>41807.03873842592</v>
+        <v>41807.88753472222</v>
       </c>
       <c r="D218" s="16" t="n">
-        <v>41807.03873842592</v>
+        <v>41807.88753472222</v>
       </c>
       <c r="E218" s="4" t="s">
         <v>8</v>
@@ -6348,16 +6348,16 @@
     </row>
     <row r="219" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B219" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C219" s="14" t="n">
-        <v>41807.04425925926</v>
+        <v>41807.888761574075</v>
       </c>
       <c r="D219" s="16" t="n">
-        <v>41807.04425925926</v>
+        <v>41807.888761574075</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F219" s="10">
         <v>0</v>
@@ -6374,16 +6374,16 @@
     </row>
     <row r="220" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B220" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C220" s="14" t="n">
-        <v>41807.04614583333</v>
+        <v>41807.907847222225</v>
       </c>
       <c r="D220" s="16" t="n">
-        <v>41807.04614583333</v>
+        <v>41807.907847222225</v>
       </c>
       <c r="E220" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F220" s="10">
         <v>0</v>
@@ -6400,16 +6400,16 @@
     </row>
     <row r="221" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C221" s="14" t="n">
-        <v>41807.0540625</v>
+        <v>41807.90828703704</v>
       </c>
       <c r="D221" s="16" t="n">
-        <v>41807.0540625</v>
+        <v>41807.90828703704</v>
       </c>
       <c r="E221" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F221" s="10">
         <v>0</v>
@@ -6426,16 +6426,16 @@
     </row>
     <row r="222" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B222" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C222" s="14" t="n">
-        <v>41807.05454861111</v>
+        <v>41807.90846064815</v>
       </c>
       <c r="D222" s="16" t="n">
-        <v>41807.05454861111</v>
+        <v>41807.90846064815</v>
       </c>
       <c r="E222" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F222" s="10">
         <v>0</v>
@@ -6452,16 +6452,16 @@
     </row>
     <row r="223" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B223" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C223" s="14" t="n">
-        <v>41807.0553125</v>
+        <v>41807.908530092594</v>
       </c>
       <c r="D223" s="16" t="n">
-        <v>41807.0553125</v>
+        <v>41807.908530092594</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="F223" s="10">
         <v>0</v>
@@ -6478,16 +6478,16 @@
     </row>
     <row r="224" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B224" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C224" s="14" t="n">
-        <v>41807.056550925925</v>
+        <v>41807.92271990741</v>
       </c>
       <c r="D224" s="16" t="n">
-        <v>41807.056550925925</v>
+        <v>41807.92271990741</v>
       </c>
       <c r="E224" s="4" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="F224" s="10">
         <v>0</v>
@@ -6504,16 +6504,16 @@
     </row>
     <row r="225" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B225" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C225" s="14" t="n">
-        <v>41807.057974537034</v>
+        <v>41807.92291666667</v>
       </c>
       <c r="D225" s="16" t="n">
-        <v>41807.057974537034</v>
+        <v>41807.92291666667</v>
       </c>
       <c r="E225" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F225" s="10">
         <v>0</v>
@@ -6530,16 +6530,16 @@
     </row>
     <row r="226" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C226" s="14" t="n">
-        <v>41807.0580787037</v>
+        <v>41807.928761574076</v>
       </c>
       <c r="D226" s="16" t="n">
-        <v>41807.0580787037</v>
+        <v>41807.928761574076</v>
       </c>
       <c r="E226" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F226" s="10">
         <v>0</v>
@@ -6556,16 +6556,16 @@
     </row>
     <row r="227" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B227" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C227" s="14" t="n">
-        <v>41807.05868055556</v>
+        <v>41807.928923611114</v>
       </c>
       <c r="D227" s="16" t="n">
-        <v>41807.05868055556</v>
+        <v>41807.928923611114</v>
       </c>
       <c r="E227" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F227" s="10">
         <v>0</v>
@@ -6585,10 +6585,10 @@
         <v>7</v>
       </c>
       <c r="C228" s="14" t="n">
-        <v>41807.06298611111</v>
+        <v>41807.93728009259</v>
       </c>
       <c r="D228" s="16" t="n">
-        <v>41807.06298611111</v>
+        <v>41807.93728009259</v>
       </c>
       <c r="E228" s="4" t="s">
         <v>8</v>
@@ -6611,13 +6611,13 @@
         <v>7</v>
       </c>
       <c r="C229" s="14" t="n">
-        <v>41807.06392361111</v>
+        <v>41807.93746527778</v>
       </c>
       <c r="D229" s="16" t="n">
-        <v>41807.06392361111</v>
+        <v>41807.93746527778</v>
       </c>
       <c r="E229" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F229" s="10">
         <v>0</v>
@@ -6637,13 +6637,13 @@
         <v>7</v>
       </c>
       <c r="C230" s="14" t="n">
-        <v>41807.06418981482</v>
+        <v>41807.94180555556</v>
       </c>
       <c r="D230" s="16" t="n">
-        <v>41807.06418981482</v>
+        <v>41807.94180555556</v>
       </c>
       <c r="E230" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F230" s="10">
         <v>0</v>
@@ -6663,13 +6663,13 @@
         <v>7</v>
       </c>
       <c r="C231" s="14" t="n">
-        <v>41807.32502314815</v>
+        <v>41807.94196759259</v>
       </c>
       <c r="D231" s="16" t="n">
-        <v>41807.32502314815</v>
+        <v>41807.94196759259</v>
       </c>
       <c r="E231" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F231" s="10">
         <v>0</v>
@@ -6689,10 +6689,10 @@
         <v>7</v>
       </c>
       <c r="C232" s="14" t="n">
-        <v>41807.879791666666</v>
+        <v>41807.94372685185</v>
       </c>
       <c r="D232" s="16" t="n">
-        <v>41807.879791666666</v>
+        <v>41807.94372685185</v>
       </c>
       <c r="E232" s="4" t="s">
         <v>8</v>
@@ -6715,13 +6715,13 @@
         <v>7</v>
       </c>
       <c r="C233" s="14" t="n">
-        <v>41807.88081018518</v>
+        <v>41807.94385416667</v>
       </c>
       <c r="D233" s="16" t="n">
-        <v>41807.88081018518</v>
+        <v>41807.94385416667</v>
       </c>
       <c r="E233" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F233" s="10">
         <v>0</v>
@@ -6738,16 +6738,16 @@
     </row>
     <row r="234" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B234" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C234" s="14" t="n">
-        <v>41807.88452546296</v>
+        <v>41807.94835648148</v>
       </c>
       <c r="D234" s="16" t="n">
-        <v>41807.88452546296</v>
+        <v>41807.94835648148</v>
       </c>
       <c r="E234" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F234" s="10">
         <v>0</v>
@@ -6767,13 +6767,13 @@
         <v>7</v>
       </c>
       <c r="C235" s="14" t="n">
-        <v>41807.88659722222</v>
+        <v>41807.94850694444</v>
       </c>
       <c r="D235" s="16" t="n">
-        <v>41807.88659722222</v>
+        <v>41807.94850694444</v>
       </c>
       <c r="E235" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F235" s="10">
         <v>0</v>
@@ -6793,13 +6793,13 @@
         <v>7</v>
       </c>
       <c r="C236" s="14" t="n">
-        <v>41807.88744212963</v>
+        <v>41807.95048611111</v>
       </c>
       <c r="D236" s="16" t="n">
-        <v>41807.88744212963</v>
+        <v>41807.95048611111</v>
       </c>
       <c r="E236" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F236" s="10">
         <v>0</v>
@@ -6819,13 +6819,13 @@
         <v>7</v>
       </c>
       <c r="C237" s="14" t="n">
-        <v>41807.88753472222</v>
+        <v>41807.95065972222</v>
       </c>
       <c r="D237" s="16" t="n">
-        <v>41807.88753472222</v>
+        <v>41807.95065972222</v>
       </c>
       <c r="E237" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F237" s="10">
         <v>0</v>
@@ -6842,16 +6842,16 @@
     </row>
     <row r="238" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B238" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C238" s="14" t="n">
-        <v>41807.888761574075</v>
+        <v>41807.965</v>
       </c>
       <c r="D238" s="16" t="n">
-        <v>41807.888761574075</v>
+        <v>41807.965</v>
       </c>
       <c r="E238" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F238" s="10">
         <v>0</v>
@@ -6868,16 +6868,16 @@
     </row>
     <row r="239" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B239" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C239" s="14" t="n">
-        <v>41807.907847222225</v>
+        <v>41807.96513888889</v>
       </c>
       <c r="D239" s="16" t="n">
-        <v>41807.907847222225</v>
+        <v>41807.96513888889</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F239" s="10">
         <v>0</v>
@@ -6897,10 +6897,10 @@
         <v>7</v>
       </c>
       <c r="C240" s="14" t="n">
-        <v>41807.90828703704</v>
+        <v>41807.966527777775</v>
       </c>
       <c r="D240" s="16" t="n">
-        <v>41807.90828703704</v>
+        <v>41807.966527777775</v>
       </c>
       <c r="E240" s="4" t="s">
         <v>8</v>
@@ -6923,13 +6923,13 @@
         <v>7</v>
       </c>
       <c r="C241" s="14" t="n">
-        <v>41807.90846064815</v>
+        <v>41807.96666666667</v>
       </c>
       <c r="D241" s="16" t="n">
-        <v>41807.90846064815</v>
+        <v>41807.96666666667</v>
       </c>
       <c r="E241" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F241" s="10">
         <v>0</v>
@@ -6949,10 +6949,10 @@
         <v>7</v>
       </c>
       <c r="C242" s="14" t="n">
-        <v>41807.908530092594</v>
+        <v>41807.97005787037</v>
       </c>
       <c r="D242" s="16" t="n">
-        <v>41807.908530092594</v>
+        <v>41807.97005787037</v>
       </c>
       <c r="E242" s="4" t="s">
         <v>8</v>
@@ -6975,13 +6975,13 @@
         <v>7</v>
       </c>
       <c r="C243" s="14" t="n">
-        <v>41807.92271990741</v>
+        <v>41807.97019675926</v>
       </c>
       <c r="D243" s="16" t="n">
-        <v>41807.92271990741</v>
+        <v>41807.97019675926</v>
       </c>
       <c r="E243" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F243" s="10">
         <v>0</v>
@@ -7001,13 +7001,13 @@
         <v>7</v>
       </c>
       <c r="C244" s="14" t="n">
-        <v>41807.92291666667</v>
+        <v>41807.97184027778</v>
       </c>
       <c r="D244" s="16" t="n">
-        <v>41807.92291666667</v>
+        <v>41807.97184027778</v>
       </c>
       <c r="E244" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F244" s="10">
         <v>0</v>
@@ -7027,13 +7027,13 @@
         <v>7</v>
       </c>
       <c r="C245" s="14" t="n">
-        <v>41807.928761574076</v>
+        <v>41807.971967592595</v>
       </c>
       <c r="D245" s="16" t="n">
-        <v>41807.928761574076</v>
+        <v>41807.971967592595</v>
       </c>
       <c r="E245" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F245" s="10">
         <v>0</v>
@@ -7053,13 +7053,13 @@
         <v>7</v>
       </c>
       <c r="C246" s="14" t="n">
-        <v>41807.928923611114</v>
+        <v>41807.97292824074</v>
       </c>
       <c r="D246" s="16" t="n">
-        <v>41807.928923611114</v>
+        <v>41807.97292824074</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F246" s="10">
         <v>0</v>
@@ -7079,10 +7079,10 @@
         <v>7</v>
       </c>
       <c r="C247" s="14" t="n">
-        <v>41807.93728009259</v>
+        <v>41808.01106481482</v>
       </c>
       <c r="D247" s="16" t="n">
-        <v>41807.93728009259</v>
+        <v>41808.01106481482</v>
       </c>
       <c r="E247" s="4" t="s">
         <v>8</v>
@@ -7105,13 +7105,13 @@
         <v>7</v>
       </c>
       <c r="C248" s="14" t="n">
-        <v>41807.93746527778</v>
+        <v>41808.01798611111</v>
       </c>
       <c r="D248" s="16" t="n">
-        <v>41807.93746527778</v>
+        <v>41808.01798611111</v>
       </c>
       <c r="E248" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F248" s="10">
         <v>0</v>
@@ -7131,10 +7131,10 @@
         <v>7</v>
       </c>
       <c r="C249" s="14" t="n">
-        <v>41807.94180555556</v>
+        <v>41808.01913194444</v>
       </c>
       <c r="D249" s="16" t="n">
-        <v>41807.94180555556</v>
+        <v>41808.01913194444</v>
       </c>
       <c r="E249" s="4" t="s">
         <v>8</v>
@@ -7157,13 +7157,13 @@
         <v>7</v>
       </c>
       <c r="C250" s="14" t="n">
-        <v>41807.94196759259</v>
+        <v>41808.01954861111</v>
       </c>
       <c r="D250" s="16" t="n">
-        <v>41807.94196759259</v>
+        <v>41808.01954861111</v>
       </c>
       <c r="E250" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F250" s="10">
         <v>0</v>
@@ -7183,10 +7183,10 @@
         <v>7</v>
       </c>
       <c r="C251" s="14" t="n">
-        <v>41807.94372685185</v>
+        <v>41808.0262037037</v>
       </c>
       <c r="D251" s="16" t="n">
-        <v>41807.94372685185</v>
+        <v>41808.0262037037</v>
       </c>
       <c r="E251" s="4" t="s">
         <v>8</v>
@@ -7209,13 +7209,13 @@
         <v>7</v>
       </c>
       <c r="C252" s="14" t="n">
-        <v>41807.94385416667</v>
+        <v>41808.026608796295</v>
       </c>
       <c r="D252" s="16" t="n">
-        <v>41807.94385416667</v>
+        <v>41808.026608796295</v>
       </c>
       <c r="E252" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F252" s="10">
         <v>0</v>
@@ -7235,10 +7235,10 @@
         <v>7</v>
       </c>
       <c r="C253" s="14" t="n">
-        <v>41807.94835648148</v>
+        <v>41808.05274305555</v>
       </c>
       <c r="D253" s="16" t="n">
-        <v>41807.94835648148</v>
+        <v>41808.05274305555</v>
       </c>
       <c r="E253" s="4" t="s">
         <v>8</v>
@@ -7261,13 +7261,13 @@
         <v>7</v>
       </c>
       <c r="C254" s="14" t="n">
-        <v>41807.94850694444</v>
+        <v>41808.053148148145</v>
       </c>
       <c r="D254" s="16" t="n">
-        <v>41807.94850694444</v>
+        <v>41808.053148148145</v>
       </c>
       <c r="E254" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F254" s="10">
         <v>0</v>
@@ -7287,10 +7287,10 @@
         <v>7</v>
       </c>
       <c r="C255" s="14" t="n">
-        <v>41807.95048611111</v>
+        <v>41809.98532407408</v>
       </c>
       <c r="D255" s="16" t="n">
-        <v>41807.95048611111</v>
+        <v>41809.98532407408</v>
       </c>
       <c r="E255" s="4" t="s">
         <v>8</v>
@@ -7313,13 +7313,13 @@
         <v>7</v>
       </c>
       <c r="C256" s="14" t="n">
-        <v>41807.95065972222</v>
+        <v>41809.98537037037</v>
       </c>
       <c r="D256" s="16" t="n">
-        <v>41807.95065972222</v>
+        <v>41809.98537037037</v>
       </c>
       <c r="E256" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F256" s="10">
         <v>0</v>
@@ -7339,10 +7339,10 @@
         <v>7</v>
       </c>
       <c r="C257" s="14" t="n">
-        <v>41807.965</v>
+        <v>41809.987222222226</v>
       </c>
       <c r="D257" s="16" t="n">
-        <v>41807.965</v>
+        <v>41809.987222222226</v>
       </c>
       <c r="E257" s="4" t="s">
         <v>8</v>
@@ -7365,13 +7365,13 @@
         <v>7</v>
       </c>
       <c r="C258" s="14" t="n">
-        <v>41807.96513888889</v>
+        <v>41809.987604166665</v>
       </c>
       <c r="D258" s="16" t="n">
-        <v>41807.96513888889</v>
+        <v>41809.987604166665</v>
       </c>
       <c r="E258" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F258" s="10">
         <v>0</v>
@@ -7391,10 +7391,10 @@
         <v>7</v>
       </c>
       <c r="C259" s="14" t="n">
-        <v>41807.966527777775</v>
+        <v>41809.98829861111</v>
       </c>
       <c r="D259" s="16" t="n">
-        <v>41807.966527777775</v>
+        <v>41809.98829861111</v>
       </c>
       <c r="E259" s="4" t="s">
         <v>8</v>
@@ -7417,13 +7417,13 @@
         <v>7</v>
       </c>
       <c r="C260" s="14" t="n">
-        <v>41807.96666666667</v>
+        <v>41809.98836805556</v>
       </c>
       <c r="D260" s="16" t="n">
-        <v>41807.96666666667</v>
+        <v>41809.98836805556</v>
       </c>
       <c r="E260" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F260" s="10">
         <v>0</v>
@@ -7443,10 +7443,10 @@
         <v>7</v>
       </c>
       <c r="C261" s="14" t="n">
-        <v>41807.97005787037</v>
+        <v>41809.99302083333</v>
       </c>
       <c r="D261" s="16" t="n">
-        <v>41807.97005787037</v>
+        <v>41809.99302083333</v>
       </c>
       <c r="E261" s="4" t="s">
         <v>8</v>
@@ -7469,13 +7469,13 @@
         <v>7</v>
       </c>
       <c r="C262" s="14" t="n">
-        <v>41807.97019675926</v>
+        <v>41809.9930787037</v>
       </c>
       <c r="D262" s="16" t="n">
-        <v>41807.97019675926</v>
+        <v>41809.9930787037</v>
       </c>
       <c r="E262" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F262" s="10">
         <v>0</v>
@@ -7495,10 +7495,10 @@
         <v>7</v>
       </c>
       <c r="C263" s="14" t="n">
-        <v>41807.97184027778</v>
+        <v>41809.99353009259</v>
       </c>
       <c r="D263" s="16" t="n">
-        <v>41807.97184027778</v>
+        <v>41809.99353009259</v>
       </c>
       <c r="E263" s="4" t="s">
         <v>8</v>
@@ -7521,13 +7521,13 @@
         <v>7</v>
       </c>
       <c r="C264" s="14" t="n">
-        <v>41807.971967592595</v>
+        <v>41809.99375</v>
       </c>
       <c r="D264" s="16" t="n">
-        <v>41807.971967592595</v>
+        <v>41809.99375</v>
       </c>
       <c r="E264" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F264" s="10">
         <v>0</v>
@@ -7547,13 +7547,13 @@
         <v>7</v>
       </c>
       <c r="C265" s="14" t="n">
-        <v>41807.97292824074</v>
+        <v>41809.993842592594</v>
       </c>
       <c r="D265" s="16" t="n">
-        <v>41807.97292824074</v>
+        <v>41809.993842592594</v>
       </c>
       <c r="E265" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F265" s="10">
         <v>0</v>
@@ -7573,13 +7573,13 @@
         <v>7</v>
       </c>
       <c r="C266" s="14" t="n">
-        <v>41808.01106481482</v>
+        <v>41809.99387731482</v>
       </c>
       <c r="D266" s="16" t="n">
-        <v>41808.01106481482</v>
+        <v>41809.99387731482</v>
       </c>
       <c r="E266" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F266" s="10">
         <v>0</v>
@@ -7599,10 +7599,10 @@
         <v>7</v>
       </c>
       <c r="C267" s="14" t="n">
-        <v>41808.01798611111</v>
+        <v>41809.99619212963</v>
       </c>
       <c r="D267" s="16" t="n">
-        <v>41808.01798611111</v>
+        <v>41809.99619212963</v>
       </c>
       <c r="E267" s="4" t="s">
         <v>8</v>
@@ -7625,13 +7625,13 @@
         <v>7</v>
       </c>
       <c r="C268" s="14" t="n">
-        <v>41808.01913194444</v>
+        <v>41809.99627314815</v>
       </c>
       <c r="D268" s="16" t="n">
-        <v>41808.01913194444</v>
+        <v>41809.99627314815</v>
       </c>
       <c r="E268" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F268" s="10">
         <v>0</v>
@@ -7651,13 +7651,13 @@
         <v>7</v>
       </c>
       <c r="C269" s="14" t="n">
-        <v>41808.01954861111</v>
+        <v>41809.996516203704</v>
       </c>
       <c r="D269" s="16" t="n">
-        <v>41808.01954861111</v>
+        <v>41809.996516203704</v>
       </c>
       <c r="E269" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F269" s="10">
         <v>0</v>
@@ -7677,13 +7677,13 @@
         <v>7</v>
       </c>
       <c r="C270" s="14" t="n">
-        <v>41808.0262037037</v>
+        <v>41809.99662037037</v>
       </c>
       <c r="D270" s="16" t="n">
-        <v>41808.0262037037</v>
+        <v>41809.99662037037</v>
       </c>
       <c r="E270" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F270" s="10">
         <v>0</v>
@@ -7703,13 +7703,13 @@
         <v>7</v>
       </c>
       <c r="C271" s="14" t="n">
-        <v>41808.026608796295</v>
+        <v>41809.99873842593</v>
       </c>
       <c r="D271" s="16" t="n">
-        <v>41808.026608796295</v>
+        <v>41809.99873842593</v>
       </c>
       <c r="E271" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F271" s="10">
         <v>0</v>
@@ -7729,13 +7729,13 @@
         <v>7</v>
       </c>
       <c r="C272" s="14" t="n">
-        <v>41808.05274305555</v>
+        <v>41809.99878472222</v>
       </c>
       <c r="D272" s="16" t="n">
-        <v>41808.05274305555</v>
+        <v>41809.99878472222</v>
       </c>
       <c r="E272" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F272" s="10">
         <v>0</v>
@@ -7755,13 +7755,13 @@
         <v>7</v>
       </c>
       <c r="C273" s="14" t="n">
-        <v>41808.053148148145</v>
+        <v>41809.99900462963</v>
       </c>
       <c r="D273" s="16" t="n">
-        <v>41808.053148148145</v>
+        <v>41809.99900462963</v>
       </c>
       <c r="E273" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F273" s="10">
         <v>0</v>
@@ -7773,500 +7773,6 @@
         <v>0</v>
       </c>
       <c r="L273" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B274" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C274" s="14" t="n">
-        <v>41809.98532407408</v>
-      </c>
-      <c r="D274" s="16" t="n">
-        <v>41809.98532407408</v>
-      </c>
-      <c r="E274" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F274" s="10">
-        <v>0</v>
-      </c>
-      <c r="H274" s="10">
-        <v>0</v>
-      </c>
-      <c r="J274" s="12">
-        <v>0</v>
-      </c>
-      <c r="L274" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B275" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C275" s="14" t="n">
-        <v>41809.98537037037</v>
-      </c>
-      <c r="D275" s="16" t="n">
-        <v>41809.98537037037</v>
-      </c>
-      <c r="E275" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F275" s="10">
-        <v>0</v>
-      </c>
-      <c r="H275" s="10">
-        <v>0</v>
-      </c>
-      <c r="J275" s="12">
-        <v>0</v>
-      </c>
-      <c r="L275" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B276" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C276" s="14" t="n">
-        <v>41809.987222222226</v>
-      </c>
-      <c r="D276" s="16" t="n">
-        <v>41809.987222222226</v>
-      </c>
-      <c r="E276" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F276" s="10">
-        <v>0</v>
-      </c>
-      <c r="H276" s="10">
-        <v>0</v>
-      </c>
-      <c r="J276" s="12">
-        <v>0</v>
-      </c>
-      <c r="L276" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B277" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C277" s="14" t="n">
-        <v>41809.987604166665</v>
-      </c>
-      <c r="D277" s="16" t="n">
-        <v>41809.987604166665</v>
-      </c>
-      <c r="E277" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F277" s="10">
-        <v>0</v>
-      </c>
-      <c r="H277" s="10">
-        <v>0</v>
-      </c>
-      <c r="J277" s="12">
-        <v>0</v>
-      </c>
-      <c r="L277" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B278" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C278" s="14" t="n">
-        <v>41809.98829861111</v>
-      </c>
-      <c r="D278" s="16" t="n">
-        <v>41809.98829861111</v>
-      </c>
-      <c r="E278" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F278" s="10">
-        <v>0</v>
-      </c>
-      <c r="H278" s="10">
-        <v>0</v>
-      </c>
-      <c r="J278" s="12">
-        <v>0</v>
-      </c>
-      <c r="L278" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B279" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C279" s="14" t="n">
-        <v>41809.98836805556</v>
-      </c>
-      <c r="D279" s="16" t="n">
-        <v>41809.98836805556</v>
-      </c>
-      <c r="E279" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F279" s="10">
-        <v>0</v>
-      </c>
-      <c r="H279" s="10">
-        <v>0</v>
-      </c>
-      <c r="J279" s="12">
-        <v>0</v>
-      </c>
-      <c r="L279" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B280" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C280" s="14" t="n">
-        <v>41809.99302083333</v>
-      </c>
-      <c r="D280" s="16" t="n">
-        <v>41809.99302083333</v>
-      </c>
-      <c r="E280" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F280" s="10">
-        <v>0</v>
-      </c>
-      <c r="H280" s="10">
-        <v>0</v>
-      </c>
-      <c r="J280" s="12">
-        <v>0</v>
-      </c>
-      <c r="L280" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B281" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C281" s="14" t="n">
-        <v>41809.9930787037</v>
-      </c>
-      <c r="D281" s="16" t="n">
-        <v>41809.9930787037</v>
-      </c>
-      <c r="E281" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F281" s="10">
-        <v>0</v>
-      </c>
-      <c r="H281" s="10">
-        <v>0</v>
-      </c>
-      <c r="J281" s="12">
-        <v>0</v>
-      </c>
-      <c r="L281" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B282" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C282" s="14" t="n">
-        <v>41809.99353009259</v>
-      </c>
-      <c r="D282" s="16" t="n">
-        <v>41809.99353009259</v>
-      </c>
-      <c r="E282" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F282" s="10">
-        <v>0</v>
-      </c>
-      <c r="H282" s="10">
-        <v>0</v>
-      </c>
-      <c r="J282" s="12">
-        <v>0</v>
-      </c>
-      <c r="L282" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B283" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C283" s="14" t="n">
-        <v>41809.99375</v>
-      </c>
-      <c r="D283" s="16" t="n">
-        <v>41809.99375</v>
-      </c>
-      <c r="E283" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F283" s="10">
-        <v>0</v>
-      </c>
-      <c r="H283" s="10">
-        <v>0</v>
-      </c>
-      <c r="J283" s="12">
-        <v>0</v>
-      </c>
-      <c r="L283" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B284" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C284" s="14" t="n">
-        <v>41809.993842592594</v>
-      </c>
-      <c r="D284" s="16" t="n">
-        <v>41809.993842592594</v>
-      </c>
-      <c r="E284" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F284" s="10">
-        <v>0</v>
-      </c>
-      <c r="H284" s="10">
-        <v>0</v>
-      </c>
-      <c r="J284" s="12">
-        <v>0</v>
-      </c>
-      <c r="L284" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B285" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C285" s="14" t="n">
-        <v>41809.99387731482</v>
-      </c>
-      <c r="D285" s="16" t="n">
-        <v>41809.99387731482</v>
-      </c>
-      <c r="E285" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F285" s="10">
-        <v>0</v>
-      </c>
-      <c r="H285" s="10">
-        <v>0</v>
-      </c>
-      <c r="J285" s="12">
-        <v>0</v>
-      </c>
-      <c r="L285" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B286" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C286" s="14" t="n">
-        <v>41809.99619212963</v>
-      </c>
-      <c r="D286" s="16" t="n">
-        <v>41809.99619212963</v>
-      </c>
-      <c r="E286" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F286" s="10">
-        <v>0</v>
-      </c>
-      <c r="H286" s="10">
-        <v>0</v>
-      </c>
-      <c r="J286" s="12">
-        <v>0</v>
-      </c>
-      <c r="L286" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B287" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C287" s="14" t="n">
-        <v>41809.99627314815</v>
-      </c>
-      <c r="D287" s="16" t="n">
-        <v>41809.99627314815</v>
-      </c>
-      <c r="E287" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F287" s="10">
-        <v>0</v>
-      </c>
-      <c r="H287" s="10">
-        <v>0</v>
-      </c>
-      <c r="J287" s="12">
-        <v>0</v>
-      </c>
-      <c r="L287" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B288" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C288" s="14" t="n">
-        <v>41809.996516203704</v>
-      </c>
-      <c r="D288" s="16" t="n">
-        <v>41809.996516203704</v>
-      </c>
-      <c r="E288" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F288" s="10">
-        <v>0</v>
-      </c>
-      <c r="H288" s="10">
-        <v>0</v>
-      </c>
-      <c r="J288" s="12">
-        <v>0</v>
-      </c>
-      <c r="L288" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B289" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C289" s="14" t="n">
-        <v>41809.99662037037</v>
-      </c>
-      <c r="D289" s="16" t="n">
-        <v>41809.99662037037</v>
-      </c>
-      <c r="E289" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F289" s="10">
-        <v>0</v>
-      </c>
-      <c r="H289" s="10">
-        <v>0</v>
-      </c>
-      <c r="J289" s="12">
-        <v>0</v>
-      </c>
-      <c r="L289" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B290" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C290" s="14" t="n">
-        <v>41809.99873842593</v>
-      </c>
-      <c r="D290" s="16" t="n">
-        <v>41809.99873842593</v>
-      </c>
-      <c r="E290" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F290" s="10">
-        <v>0</v>
-      </c>
-      <c r="H290" s="10">
-        <v>0</v>
-      </c>
-      <c r="J290" s="12">
-        <v>0</v>
-      </c>
-      <c r="L290" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B291" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C291" s="14" t="n">
-        <v>41809.99878472222</v>
-      </c>
-      <c r="D291" s="16" t="n">
-        <v>41809.99878472222</v>
-      </c>
-      <c r="E291" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F291" s="10">
-        <v>0</v>
-      </c>
-      <c r="H291" s="10">
-        <v>0</v>
-      </c>
-      <c r="J291" s="12">
-        <v>0</v>
-      </c>
-      <c r="L291" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B292" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C292" s="14" t="n">
-        <v>41809.99900462963</v>
-      </c>
-      <c r="D292" s="16" t="n">
-        <v>41809.99900462963</v>
-      </c>
-      <c r="E292" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F292" s="10">
-        <v>0</v>
-      </c>
-      <c r="H292" s="10">
-        <v>0</v>
-      </c>
-      <c r="J292" s="12">
-        <v>0</v>
-      </c>
-      <c r="L292" s="4" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>